<commit_message>
scrap debug and python only
</commit_message>
<xml_diff>
--- a/code/data_scrap/downloads/exchange_rate/exchange_rates.xlsx
+++ b/code/data_scrap/downloads/exchange_rate/exchange_rates.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D281"/>
+  <dimension ref="A1:D282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
         <v>36738</v>
       </c>
       <c r="B2" t="n">
-        <v>1.557932637480509</v>
+        <v>1.557932622301237</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
@@ -478,7 +478,7 @@
         <v>36769</v>
       </c>
       <c r="B3" t="n">
-        <v>1.564211900105158</v>
+        <v>1.564211843535298</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
@@ -490,7 +490,7 @@
         <v>36799</v>
       </c>
       <c r="B4" t="n">
-        <v>1.555621164184631</v>
+        <v>1.555621076070142</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
@@ -502,7 +502,7 @@
         <v>36830</v>
       </c>
       <c r="B5" t="n">
-        <v>1.558262791060175</v>
+        <v>1.558262805296498</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
@@ -514,7 +514,7 @@
         <v>36860</v>
       </c>
       <c r="B6" t="n">
-        <v>1.553083723495852</v>
+        <v>1.553083859687902</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
@@ -526,7 +526,7 @@
         <v>36891</v>
       </c>
       <c r="B7" t="n">
-        <v>1.548356844345664</v>
+        <v>1.548356842256252</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
@@ -538,7 +538,7 @@
         <v>36922</v>
       </c>
       <c r="B8" t="n">
-        <v>1.55120104132816</v>
+        <v>1.551200928651912</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
@@ -550,7 +550,7 @@
         <v>36950</v>
       </c>
       <c r="B9" t="n">
-        <v>1.551460499094336</v>
+        <v>1.551460474499731</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
@@ -562,7 +562,7 @@
         <v>36981</v>
       </c>
       <c r="B10" t="n">
-        <v>1.542570419084366</v>
+        <v>1.542570421997034</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
@@ -574,7 +574,7 @@
         <v>37011</v>
       </c>
       <c r="B11" t="n">
-        <v>1.523479363440448</v>
+        <v>1.523479342697656</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
@@ -586,7 +586,7 @@
         <v>37042</v>
       </c>
       <c r="B12" t="n">
-        <v>1.524239660512331</v>
+        <v>1.524239509652734</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
@@ -598,7 +598,7 @@
         <v>37072</v>
       </c>
       <c r="B13" t="n">
-        <v>1.528944406227523</v>
+        <v>1.528944441360265</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
@@ -610,13 +610,13 @@
         <v>37103</v>
       </c>
       <c r="B14" t="n">
-        <v>1.534972025173091</v>
+        <v>1.534971993001763</v>
       </c>
       <c r="C14" t="n">
         <v>0.9987750053405762</v>
       </c>
       <c r="D14" t="n">
-        <v>1.318850785584947</v>
+        <v>1.318850663777466</v>
       </c>
     </row>
     <row r="15">
@@ -624,13 +624,13 @@
         <v>37134</v>
       </c>
       <c r="B15" t="n">
-        <v>1.551573095697607</v>
+        <v>1.551573230504147</v>
       </c>
       <c r="C15" t="n">
         <v>0.9987374991178513</v>
       </c>
       <c r="D15" t="n">
-        <v>1.565736663375915</v>
+        <v>1.565736914716247</v>
       </c>
     </row>
     <row r="16">
@@ -638,13 +638,13 @@
         <v>37164</v>
       </c>
       <c r="B16" t="n">
-        <v>1.616362236225483</v>
+        <v>1.616362264332305</v>
       </c>
       <c r="C16" t="n">
         <v>0.9984500110149384</v>
       </c>
       <c r="D16" t="n">
-        <v>1.587020962979894</v>
+        <v>1.587020931729439</v>
       </c>
     </row>
     <row r="17">
@@ -652,11 +652,11 @@
         <v>37195</v>
       </c>
       <c r="B17" t="n">
-        <v>1.586766300445286</v>
+        <v>1.586766341399618</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>1.595669051334342</v>
+        <v>1.595669054192186</v>
       </c>
     </row>
     <row r="18">
@@ -664,11 +664,11 @@
         <v>37225</v>
       </c>
       <c r="B18" t="n">
-        <v>1.523182996516333</v>
+        <v>1.523183099942531</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>1.595669051334342</v>
+        <v>1.595669054192186</v>
       </c>
     </row>
     <row r="19">
@@ -676,11 +676,11 @@
         <v>37256</v>
       </c>
       <c r="B19" t="n">
-        <v>1.526998181343102</v>
+        <v>1.526998295681875</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>1.595669051334342</v>
+        <v>1.595669054192186</v>
       </c>
     </row>
     <row r="20">
@@ -688,11 +688,11 @@
         <v>37287</v>
       </c>
       <c r="B20" t="n">
-        <v>1.80573223305065</v>
+        <v>1.8057322147671</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>1.595669051334342</v>
+        <v>1.595669054192186</v>
       </c>
     </row>
     <row r="21">
@@ -700,11 +700,11 @@
         <v>37315</v>
       </c>
       <c r="B21" t="n">
-        <v>3.261907229846081</v>
+        <v>3.261907376343026</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1.595669051334342</v>
+        <v>1.595669054192186</v>
       </c>
     </row>
     <row r="22">
@@ -712,11 +712,11 @@
         <v>37346</v>
       </c>
       <c r="B22" t="n">
-        <v>3.810694782289236</v>
+        <v>3.810694429781901</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>1.595669051334342</v>
+        <v>1.595669054192186</v>
       </c>
     </row>
     <row r="23">
@@ -724,13 +724,13 @@
         <v>37376</v>
       </c>
       <c r="B23" t="n">
-        <v>4.614307962258205</v>
+        <v>4.61430786724955</v>
       </c>
       <c r="C23" t="n">
         <v>2.977142878941127</v>
       </c>
       <c r="D23" t="n">
-        <v>1.499912157948904</v>
+        <v>1.49991217566771</v>
       </c>
     </row>
     <row r="24">
@@ -738,13 +738,13 @@
         <v>37407</v>
       </c>
       <c r="B24" t="n">
-        <v>5.128639915648731</v>
+        <v>5.128640033614506</v>
       </c>
       <c r="C24" t="n">
         <v>3.393750011920929</v>
       </c>
       <c r="D24" t="n">
-        <v>1.513420105516485</v>
+        <v>1.513420306337874</v>
       </c>
     </row>
     <row r="25">
@@ -752,13 +752,13 @@
         <v>37437</v>
       </c>
       <c r="B25" t="n">
-        <v>5.778270675178004</v>
+        <v>5.778270972580831</v>
       </c>
       <c r="C25" t="n">
         <v>3.652499973773956</v>
       </c>
       <c r="D25" t="n">
-        <v>1.625817940533744</v>
+        <v>1.625818126312785</v>
       </c>
     </row>
     <row r="26">
@@ -766,13 +766,13 @@
         <v>37468</v>
       </c>
       <c r="B26" t="n">
-        <v>5.495428023323131</v>
+        <v>5.495427805884704</v>
       </c>
       <c r="C26" t="n">
         <v>3.653333266576131</v>
       </c>
       <c r="D26" t="n">
-        <v>1.512234918584395</v>
+        <v>1.512234766406683</v>
       </c>
     </row>
     <row r="27">
@@ -780,13 +780,13 @@
         <v>37499</v>
       </c>
       <c r="B27" t="n">
-        <v>5.458250735003496</v>
+        <v>5.45825068330661</v>
       </c>
       <c r="C27" t="n">
         <v>3.626249969005585</v>
       </c>
       <c r="D27" t="n">
-        <v>1.454831948160072</v>
+        <v>1.454831814574389</v>
       </c>
     </row>
     <row r="28">
@@ -794,13 +794,13 @@
         <v>37529</v>
       </c>
       <c r="B28" t="n">
-        <v>5.633745061845254</v>
+        <v>5.633745237623661</v>
       </c>
       <c r="C28" t="n">
         <v>3.664999961853027</v>
       </c>
       <c r="D28" t="n">
-        <v>1.505223163487753</v>
+        <v>1.505222968995642</v>
       </c>
     </row>
     <row r="29">
@@ -808,13 +808,13 @@
         <v>37560</v>
       </c>
       <c r="B29" t="n">
-        <v>5.813316882678887</v>
+        <v>5.813317064109442</v>
       </c>
       <c r="C29" t="n">
         <v>3.680000007152557</v>
       </c>
       <c r="D29" t="n">
-        <v>1.594659358602862</v>
+        <v>1.59465950418561</v>
       </c>
     </row>
     <row r="30">
@@ -822,13 +822,13 @@
         <v>37590</v>
       </c>
       <c r="B30" t="n">
-        <v>5.297231969943631</v>
+        <v>5.297231774399285</v>
       </c>
       <c r="C30" t="n">
         <v>3.56166672706604</v>
       </c>
       <c r="D30" t="n">
-        <v>1.483493579890309</v>
+        <v>1.483493335952399</v>
       </c>
     </row>
     <row r="31">
@@ -836,13 +836,13 @@
         <v>37621</v>
       </c>
       <c r="B31" t="n">
-        <v>4.84088928863439</v>
+        <v>4.840888996753685</v>
       </c>
       <c r="C31" t="n">
         <v>3.5</v>
       </c>
       <c r="D31" t="n">
-        <v>1.36418554049134</v>
+        <v>1.364185426517679</v>
       </c>
     </row>
     <row r="32">
@@ -850,13 +850,13 @@
         <v>37652</v>
       </c>
       <c r="B32" t="n">
-        <v>4.420961938355728</v>
+        <v>4.420962099337777</v>
       </c>
       <c r="C32" t="n">
         <v>3.309000015258789</v>
       </c>
       <c r="D32" t="n">
-        <v>1.327694514399035</v>
+        <v>1.32769461449558</v>
       </c>
     </row>
     <row r="33">
@@ -864,13 +864,13 @@
         <v>37680</v>
       </c>
       <c r="B33" t="n">
-        <v>4.273359104656306</v>
+        <v>4.273359390211739</v>
       </c>
       <c r="C33" t="n">
         <v>3.169999957084656</v>
       </c>
       <c r="D33" t="n">
-        <v>1.358876256721226</v>
+        <v>1.358876443327064</v>
       </c>
     </row>
     <row r="34">
@@ -878,13 +878,13 @@
         <v>37711</v>
       </c>
       <c r="B34" t="n">
-        <v>4.148074399177069</v>
+        <v>4.148074163966041</v>
       </c>
       <c r="C34" t="n">
         <v>3.11214280128479</v>
       </c>
       <c r="D34" t="n">
-        <v>1.35545388990755</v>
+        <v>1.355453721857792</v>
       </c>
     </row>
     <row r="35">
@@ -892,13 +892,13 @@
         <v>37741</v>
       </c>
       <c r="B35" t="n">
-        <v>3.774657322702299</v>
+        <v>3.774657442902706</v>
       </c>
       <c r="C35" t="n">
         <v>2.904999971389771</v>
       </c>
       <c r="D35" t="n">
-        <v>1.319050167450333</v>
+        <v>1.31905021772146</v>
       </c>
     </row>
     <row r="36">
@@ -906,11 +906,11 @@
         <v>37772</v>
       </c>
       <c r="B36" t="n">
-        <v>3.578751363698895</v>
+        <v>3.578751121376695</v>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>1.229504604401884</v>
+        <v>1.229504710947705</v>
       </c>
     </row>
     <row r="37">
@@ -918,11 +918,11 @@
         <v>37802</v>
       </c>
       <c r="B37" t="n">
-        <v>3.544311044173685</v>
+        <v>3.544310999998202</v>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
-        <v>1.229504604401884</v>
+        <v>1.229504710947705</v>
       </c>
     </row>
     <row r="38">
@@ -930,11 +930,11 @@
         <v>37833</v>
       </c>
       <c r="B38" t="n">
-        <v>3.507977667836236</v>
+        <v>3.507977741277413</v>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="n">
-        <v>1.229504604401884</v>
+        <v>1.229504710947705</v>
       </c>
     </row>
     <row r="39">
@@ -942,11 +942,11 @@
         <v>37864</v>
       </c>
       <c r="B39" t="n">
-        <v>3.640920253326037</v>
+        <v>3.640920474995185</v>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
-        <v>1.229504604401884</v>
+        <v>1.229504710947705</v>
       </c>
     </row>
     <row r="40">
@@ -954,11 +954,11 @@
         <v>37894</v>
       </c>
       <c r="B40" t="n">
-        <v>3.619666434968427</v>
+        <v>3.619666591707389</v>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
-        <v>1.229504604401884</v>
+        <v>1.229504710947705</v>
       </c>
     </row>
     <row r="41">
@@ -966,11 +966,11 @@
         <v>37925</v>
       </c>
       <c r="B41" t="n">
-        <v>3.516867045239735</v>
+        <v>3.516867168487289</v>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="n">
-        <v>1.229504604401884</v>
+        <v>1.229504710947705</v>
       </c>
     </row>
     <row r="42">
@@ -978,11 +978,11 @@
         <v>37955</v>
       </c>
       <c r="B42" t="n">
-        <v>3.549792143101043</v>
+        <v>3.54979200795155</v>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
-        <v>1.229504604401884</v>
+        <v>1.229504710947705</v>
       </c>
     </row>
     <row r="43">
@@ -990,13 +990,13 @@
         <v>37986</v>
       </c>
       <c r="B43" t="n">
-        <v>3.633174408938393</v>
+        <v>3.633174491506801</v>
       </c>
       <c r="C43" t="n">
         <v>2.92231502532959</v>
       </c>
       <c r="D43" t="n">
-        <v>1.24327126661763</v>
+        <v>1.24327127502373</v>
       </c>
     </row>
     <row r="44">
@@ -1004,13 +1004,13 @@
         <v>38017</v>
       </c>
       <c r="B44" t="n">
-        <v>3.59134922723442</v>
+        <v>3.591349270752813</v>
       </c>
       <c r="C44" t="n">
         <v>2.854390473592849</v>
       </c>
       <c r="D44" t="n">
-        <v>1.25773594173035</v>
+        <v>1.257735951752051</v>
       </c>
     </row>
     <row r="45">
@@ -1018,13 +1018,13 @@
         <v>38046</v>
       </c>
       <c r="B45" t="n">
-        <v>3.597301427486496</v>
+        <v>3.597301831380817</v>
       </c>
       <c r="C45" t="n">
         <v>2.88683500289917</v>
       </c>
       <c r="D45" t="n">
-        <v>1.246255543031876</v>
+        <v>1.24625568241965</v>
       </c>
     </row>
     <row r="46">
@@ -1032,13 +1032,13 @@
         <v>38077</v>
       </c>
       <c r="B46" t="n">
-        <v>3.566499611082259</v>
+        <v>3.566499390699375</v>
       </c>
       <c r="C46" t="n">
         <v>2.862786946089372</v>
       </c>
       <c r="D46" t="n">
-        <v>1.245766774444829</v>
+        <v>1.245766697406752</v>
       </c>
     </row>
     <row r="47">
@@ -1046,13 +1046,13 @@
         <v>38107</v>
       </c>
       <c r="B47" t="n">
-        <v>3.425917414153565</v>
+        <v>3.425917691086157</v>
       </c>
       <c r="C47" t="n">
         <v>2.798489999771118</v>
       </c>
       <c r="D47" t="n">
-        <v>1.225265820227241</v>
+        <v>1.225265913854983</v>
       </c>
     </row>
     <row r="48">
@@ -1060,13 +1060,13 @@
         <v>38138</v>
       </c>
       <c r="B48" t="n">
-        <v>3.433667005020236</v>
+        <v>3.433667049093757</v>
       </c>
       <c r="C48" t="n">
         <v>2.859205233423333</v>
       </c>
       <c r="D48" t="n">
-        <v>1.19926320765198</v>
+        <v>1.199263223288605</v>
       </c>
     </row>
     <row r="49">
@@ -1074,13 +1074,13 @@
         <v>38168</v>
       </c>
       <c r="B49" t="n">
-        <v>3.475856536931476</v>
+        <v>3.475856567282692</v>
       </c>
       <c r="C49" t="n">
         <v>2.923018184575167</v>
       </c>
       <c r="D49" t="n">
-        <v>1.189153707327946</v>
+        <v>1.189153717780608</v>
       </c>
     </row>
     <row r="50">
@@ -1088,13 +1088,13 @@
         <v>38199</v>
       </c>
       <c r="B50" t="n">
-        <v>3.45923806777967</v>
+        <v>3.4592384362916</v>
       </c>
       <c r="C50" t="n">
         <v>2.917272730307146</v>
       </c>
       <c r="D50" t="n">
-        <v>1.185787139190701</v>
+        <v>1.185787265644597</v>
       </c>
     </row>
     <row r="51">
@@ -1102,13 +1102,13 @@
         <v>38230</v>
       </c>
       <c r="B51" t="n">
-        <v>3.527178557916964</v>
+        <v>3.527178584952339</v>
       </c>
       <c r="C51" t="n">
         <v>2.959840915419839</v>
       </c>
       <c r="D51" t="n">
-        <v>1.191746124851182</v>
+        <v>1.191746134277562</v>
       </c>
     </row>
     <row r="52">
@@ -1116,13 +1116,13 @@
         <v>38260</v>
       </c>
       <c r="B52" t="n">
-        <v>3.4966461302805</v>
+        <v>3.496646184781531</v>
       </c>
       <c r="C52" t="n">
         <v>2.959086363965815</v>
       </c>
       <c r="D52" t="n">
-        <v>1.181667662972088</v>
+        <v>1.181667681630981</v>
       </c>
     </row>
     <row r="53">
@@ -1130,13 +1130,13 @@
         <v>38291</v>
       </c>
       <c r="B53" t="n">
-        <v>3.472415608395341</v>
+        <v>3.472415715836689</v>
       </c>
       <c r="C53" t="n">
         <v>2.947190466381254</v>
       </c>
       <c r="D53" t="n">
-        <v>1.17824838279612</v>
+        <v>1.178248419116822</v>
       </c>
     </row>
     <row r="54">
@@ -1144,13 +1144,13 @@
         <v>38321</v>
       </c>
       <c r="B54" t="n">
-        <v>3.361466340306317</v>
+        <v>3.361466320116946</v>
       </c>
       <c r="C54" t="n">
         <v>2.949068199504505</v>
       </c>
       <c r="D54" t="n">
-        <v>1.13984945331076</v>
+        <v>1.139849446903489</v>
       </c>
     </row>
     <row r="55">
@@ -1158,13 +1158,13 @@
         <v>38352</v>
       </c>
       <c r="B55" t="n">
-        <v>3.386270218040695</v>
+        <v>3.386270351869677</v>
       </c>
       <c r="C55" t="n">
         <v>2.962021755135578</v>
       </c>
       <c r="D55" t="n">
-        <v>1.143252296862882</v>
+        <v>1.14325234193612</v>
       </c>
     </row>
     <row r="56">
@@ -1172,13 +1172,13 @@
         <v>38383</v>
       </c>
       <c r="B56" t="n">
-        <v>3.373987884519517</v>
+        <v>3.373987816847431</v>
       </c>
       <c r="C56" t="n">
         <v>2.922652380807059</v>
       </c>
       <c r="D56" t="n">
-        <v>1.154716721464261</v>
+        <v>1.154716697670655</v>
       </c>
     </row>
     <row r="57">
@@ -1186,13 +1186,13 @@
         <v>38411</v>
       </c>
       <c r="B57" t="n">
-        <v>3.331415880993684</v>
+        <v>3.331415975762798</v>
       </c>
       <c r="C57" t="n">
         <v>2.871909987926483</v>
       </c>
       <c r="D57" t="n">
-        <v>1.160476931260005</v>
+        <v>1.160476962885349</v>
       </c>
     </row>
     <row r="58">
@@ -1200,13 +1200,13 @@
         <v>38442</v>
       </c>
       <c r="B58" t="n">
-        <v>3.365121713016211</v>
+        <v>3.365121882638827</v>
       </c>
       <c r="C58" t="n">
         <v>2.877030424449755</v>
       </c>
       <c r="D58" t="n">
-        <v>1.170061480488451</v>
+        <v>1.170061538395163</v>
       </c>
     </row>
     <row r="59">
@@ -1214,13 +1214,13 @@
         <v>38472</v>
       </c>
       <c r="B59" t="n">
-        <v>3.330682673799504</v>
+        <v>3.330682718255194</v>
       </c>
       <c r="C59" t="n">
         <v>2.898761930919829</v>
       </c>
       <c r="D59" t="n">
-        <v>1.149007851051184</v>
+        <v>1.149007866566784</v>
       </c>
     </row>
     <row r="60">
@@ -1228,13 +1228,13 @@
         <v>38503</v>
       </c>
       <c r="B60" t="n">
-        <v>3.239534973806319</v>
+        <v>3.239534913569946</v>
       </c>
       <c r="C60" t="n">
         <v>2.888272697275335</v>
       </c>
       <c r="D60" t="n">
-        <v>1.121608587667254</v>
+        <v>1.121608566652618</v>
       </c>
     </row>
     <row r="61">
@@ -1242,13 +1242,13 @@
         <v>38533</v>
       </c>
       <c r="B61" t="n">
-        <v>3.19140946615973</v>
+        <v>3.191409366853301</v>
       </c>
       <c r="C61" t="n">
         <v>2.875459064136852</v>
       </c>
       <c r="D61" t="n">
-        <v>1.109963600602293</v>
+        <v>1.109963566004309</v>
       </c>
     </row>
     <row r="62">
@@ -1256,13 +1256,13 @@
         <v>38564</v>
       </c>
       <c r="B62" t="n">
-        <v>3.165867030619235</v>
+        <v>3.165867060858524</v>
       </c>
       <c r="C62" t="n">
         <v>2.86738091423398</v>
       </c>
       <c r="D62" t="n">
-        <v>1.104104713658065</v>
+        <v>1.104104724116657</v>
       </c>
     </row>
     <row r="63">
@@ -1270,13 +1270,13 @@
         <v>38595</v>
       </c>
       <c r="B63" t="n">
-        <v>3.192260589880004</v>
+        <v>3.192260658123995</v>
       </c>
       <c r="C63" t="n">
         <v>2.880230468252431</v>
       </c>
       <c r="D63" t="n">
-        <v>1.108396229601597</v>
+        <v>1.108396253137764</v>
       </c>
     </row>
     <row r="64">
@@ -1284,13 +1284,13 @@
         <v>38625</v>
       </c>
       <c r="B64" t="n">
-        <v>3.229578278877327</v>
+        <v>3.229578179098772</v>
       </c>
       <c r="C64" t="n">
         <v>2.903170455585827</v>
       </c>
       <c r="D64" t="n">
-        <v>1.112568434679834</v>
+        <v>1.112568400417228</v>
       </c>
     </row>
     <row r="65">
@@ -1298,13 +1298,13 @@
         <v>38656</v>
       </c>
       <c r="B65" t="n">
-        <v>3.304905594612257</v>
+        <v>3.304905580764699</v>
       </c>
       <c r="C65" t="n">
         <v>2.965595234008062</v>
       </c>
       <c r="D65" t="n">
-        <v>1.114354227016314</v>
+        <v>1.114354222263284</v>
       </c>
     </row>
     <row r="66">
@@ -1312,13 +1312,13 @@
         <v>38686</v>
       </c>
       <c r="B66" t="n">
-        <v>3.284334934984527</v>
+        <v>3.284334716779166</v>
       </c>
       <c r="C66" t="n">
         <v>2.963172728365118</v>
       </c>
       <c r="D66" t="n">
-        <v>1.108391868060511</v>
+        <v>1.10839179396216</v>
       </c>
     </row>
     <row r="67">
@@ -1326,13 +1326,13 @@
         <v>38717</v>
       </c>
       <c r="B67" t="n">
-        <v>3.339521790190866</v>
+        <v>3.3395219263409</v>
       </c>
       <c r="C67" t="n">
         <v>3.011345440691167</v>
       </c>
       <c r="D67" t="n">
-        <v>1.108932708148006</v>
+        <v>1.108932753226114</v>
       </c>
     </row>
     <row r="68">
@@ -1340,13 +1340,13 @@
         <v>38748</v>
       </c>
       <c r="B68" t="n">
-        <v>3.389294577314663</v>
+        <v>3.389294708333836</v>
       </c>
       <c r="C68" t="n">
         <v>3.046218167651783</v>
       </c>
       <c r="D68" t="n">
-        <v>1.11261549429263</v>
+        <v>1.112615537286972</v>
       </c>
     </row>
     <row r="69">
@@ -1354,13 +1354,13 @@
         <v>38776</v>
       </c>
       <c r="B69" t="n">
-        <v>3.365425689771121</v>
+        <v>3.365425833851507</v>
       </c>
       <c r="C69" t="n">
         <v>3.06855001449585</v>
       </c>
       <c r="D69" t="n">
-        <v>1.096749229802299</v>
+        <v>1.096749276734987</v>
       </c>
     </row>
     <row r="70">
@@ -1368,13 +1368,13 @@
         <v>38807</v>
       </c>
       <c r="B70" t="n">
-        <v>3.348461987480988</v>
+        <v>3.348462011906954</v>
       </c>
       <c r="C70" t="n">
         <v>3.062952155652253</v>
       </c>
       <c r="D70" t="n">
-        <v>1.093387925578673</v>
+        <v>1.093387933283368</v>
       </c>
     </row>
     <row r="71">
@@ -1382,13 +1382,13 @@
         <v>38837</v>
       </c>
       <c r="B71" t="n">
-        <v>3.325859773743575</v>
+        <v>3.325859716015879</v>
       </c>
       <c r="C71" t="n">
         <v>3.014434969425202</v>
       </c>
       <c r="D71" t="n">
-        <v>1.103752391537128</v>
+        <v>1.103752372412346</v>
       </c>
     </row>
     <row r="72">
@@ -1396,13 +1396,13 @@
         <v>38868</v>
       </c>
       <c r="B72" t="n">
-        <v>3.273039102882895</v>
+        <v>3.273039220159847</v>
       </c>
       <c r="C72" t="n">
         <v>3.051456534344217</v>
       </c>
       <c r="D72" t="n">
-        <v>1.072605215958221</v>
+        <v>1.072605254467057</v>
       </c>
     </row>
     <row r="73">
@@ -1410,13 +1410,13 @@
         <v>38898</v>
       </c>
       <c r="B73" t="n">
-        <v>3.343030095705292</v>
+        <v>3.343030198512139</v>
       </c>
       <c r="C73" t="n">
         <v>3.076404582370411</v>
       </c>
       <c r="D73" t="n">
-        <v>1.086673681610881</v>
+        <v>1.08667371501072</v>
       </c>
     </row>
     <row r="74">
@@ -1424,13 +1424,13 @@
         <v>38929</v>
       </c>
       <c r="B74" t="n">
-        <v>3.297140023103178</v>
+        <v>3.29714022078047</v>
       </c>
       <c r="C74" t="n">
         <v>3.077495245706467</v>
       </c>
       <c r="D74" t="n">
-        <v>1.071373224308062</v>
+        <v>1.071373288468155</v>
       </c>
     </row>
     <row r="75">
@@ -1438,13 +1438,13 @@
         <v>38960</v>
       </c>
       <c r="B75" t="n">
-        <v>3.310192428968088</v>
+        <v>3.310192539797054</v>
       </c>
       <c r="C75" t="n">
         <v>3.070482606473176</v>
       </c>
       <c r="D75" t="n">
-        <v>1.078135094197441</v>
+        <v>1.078135130212329</v>
       </c>
     </row>
     <row r="76">
@@ -1452,13 +1452,13 @@
         <v>38990</v>
       </c>
       <c r="B76" t="n">
-        <v>3.299602591197812</v>
+        <v>3.29960252658127</v>
       </c>
       <c r="C76" t="n">
         <v>3.095476184572493</v>
       </c>
       <c r="D76" t="n">
-        <v>1.065943107887092</v>
+        <v>1.065943087047382</v>
       </c>
     </row>
     <row r="77">
@@ -1466,13 +1466,13 @@
         <v>39021</v>
       </c>
       <c r="B77" t="n">
-        <v>3.309117021576025</v>
+        <v>3.309117081037666</v>
       </c>
       <c r="C77" t="n">
         <v>3.094300020824779</v>
       </c>
       <c r="D77" t="n">
-        <v>1.069429206883925</v>
+        <v>1.069429226152336</v>
       </c>
     </row>
     <row r="78">
@@ -1480,13 +1480,13 @@
         <v>39051</v>
       </c>
       <c r="B78" t="n">
-        <v>3.296785445894844</v>
+        <v>3.296785291867417</v>
       </c>
       <c r="C78" t="n">
         <v>3.070981838486411</v>
       </c>
       <c r="D78" t="n">
-        <v>1.073521967716239</v>
+        <v>1.073521917545254</v>
       </c>
     </row>
     <row r="79">
@@ -1494,13 +1494,13 @@
         <v>39082</v>
       </c>
       <c r="B79" t="n">
-        <v>3.224508105823276</v>
+        <v>3.224508273289052</v>
       </c>
       <c r="C79" t="n">
         <v>3.053995245978946</v>
       </c>
       <c r="D79" t="n">
-        <v>1.055480747254855</v>
+        <v>1.055480805608078</v>
       </c>
     </row>
     <row r="80">
@@ -1508,13 +1508,13 @@
         <v>39113</v>
       </c>
       <c r="B80" t="n">
-        <v>3.264375584567959</v>
+        <v>3.264375574545679</v>
       </c>
       <c r="C80" t="n">
         <v>3.079639144565748</v>
       </c>
       <c r="D80" t="n">
-        <v>1.059581963378814</v>
+        <v>1.059581947031883</v>
       </c>
     </row>
     <row r="81">
@@ -1522,13 +1522,13 @@
         <v>39141</v>
       </c>
       <c r="B81" t="n">
-        <v>3.293526409415832</v>
+        <v>3.293526493512716</v>
       </c>
       <c r="C81" t="n">
         <v>3.097704994678497</v>
       </c>
       <c r="D81" t="n">
-        <v>1.063216135602114</v>
+        <v>1.063216162762246</v>
       </c>
     </row>
     <row r="82">
@@ -1536,13 +1536,13 @@
         <v>39172</v>
       </c>
       <c r="B82" t="n">
-        <v>3.276466052363151</v>
+        <v>3.276465944330631</v>
       </c>
       <c r="C82" t="n">
         <v>3.096545468677174</v>
       </c>
       <c r="D82" t="n">
-        <v>1.058107280579988</v>
+        <v>1.058107245713506</v>
       </c>
     </row>
     <row r="83">
@@ -1550,13 +1550,13 @@
         <v>39202</v>
       </c>
       <c r="B83" t="n">
-        <v>3.215239785720839</v>
+        <v>3.215239583220978</v>
       </c>
       <c r="C83" t="n">
         <v>3.086199998855591</v>
       </c>
       <c r="D83" t="n">
-        <v>1.041967952649182</v>
+        <v>1.041967880813256</v>
       </c>
     </row>
     <row r="84">
@@ -1564,13 +1564,13 @@
         <v>39233</v>
       </c>
       <c r="B84" t="n">
-        <v>3.213103661305728</v>
+        <v>3.213103695646243</v>
       </c>
       <c r="C84" t="n">
         <v>3.076591325842816</v>
       </c>
       <c r="D84" t="n">
-        <v>1.044372239764431</v>
+        <v>1.044372250929271</v>
       </c>
     </row>
     <row r="85">
@@ -1578,13 +1578,13 @@
         <v>39263</v>
       </c>
       <c r="B85" t="n">
-        <v>3.216856094011028</v>
+        <v>3.216856182628796</v>
       </c>
       <c r="C85" t="n">
         <v>3.075661897659302</v>
       </c>
       <c r="D85" t="n">
-        <v>1.045901825386781</v>
+        <v>1.045901854198781</v>
       </c>
     </row>
     <row r="86">
@@ -1592,13 +1592,13 @@
         <v>39294</v>
       </c>
       <c r="B86" t="n">
-        <v>3.286914559025071</v>
+        <v>3.286914443268888</v>
       </c>
       <c r="C86" t="n">
         <v>3.107786362821406</v>
       </c>
       <c r="D86" t="n">
-        <v>1.057596644953511</v>
+        <v>1.057596607888466</v>
       </c>
     </row>
     <row r="87">
@@ -1606,13 +1606,13 @@
         <v>39325</v>
       </c>
       <c r="B87" t="n">
-        <v>3.349284428649809</v>
+        <v>3.349284547162641</v>
       </c>
       <c r="C87" t="n">
         <v>3.150747796763544</v>
       </c>
       <c r="D87" t="n">
-        <v>1.063039627092685</v>
+        <v>1.063039664683142</v>
       </c>
     </row>
     <row r="88">
@@ -1620,13 +1620,13 @@
         <v>39355</v>
       </c>
       <c r="B88" t="n">
-        <v>3.406868293548255</v>
+        <v>3.406868418118327</v>
       </c>
       <c r="C88" t="n">
         <v>3.141869986057281</v>
       </c>
       <c r="D88" t="n">
-        <v>1.084317053273673</v>
+        <v>1.084317092894268</v>
       </c>
     </row>
     <row r="89">
@@ -1634,13 +1634,13 @@
         <v>39386</v>
       </c>
       <c r="B89" t="n">
-        <v>3.340131549434752</v>
+        <v>3.340131593220602</v>
       </c>
       <c r="C89" t="n">
         <v>3.153552179751189</v>
       </c>
       <c r="D89" t="n">
-        <v>1.059182120291749</v>
+        <v>1.059182134261885</v>
       </c>
     </row>
     <row r="90">
@@ -1648,13 +1648,13 @@
         <v>39416</v>
       </c>
       <c r="B90" t="n">
-        <v>3.333647505435213</v>
+        <v>3.333647543613205</v>
       </c>
       <c r="C90" t="n">
         <v>3.132481835105203</v>
       </c>
       <c r="D90" t="n">
-        <v>1.064223483778122</v>
+        <v>1.064223496029524</v>
       </c>
     </row>
     <row r="91">
@@ -1662,13 +1662,13 @@
         <v>39447</v>
       </c>
       <c r="B91" t="n">
-        <v>3.305624581759615</v>
+        <v>3.305624713403216</v>
       </c>
       <c r="C91" t="n">
         <v>3.129476195289975</v>
       </c>
       <c r="D91" t="n">
-        <v>1.056656732089259</v>
+        <v>1.05665677363854</v>
       </c>
     </row>
     <row r="92">
@@ -1676,13 +1676,13 @@
         <v>39478</v>
       </c>
       <c r="B92" t="n">
-        <v>3.342189330266241</v>
+        <v>3.342189430697698</v>
       </c>
       <c r="C92" t="n">
         <v>3.142186921575795</v>
       </c>
       <c r="D92" t="n">
-        <v>1.063034670547801</v>
+        <v>1.063034709171409</v>
       </c>
     </row>
     <row r="93">
@@ -1690,13 +1690,13 @@
         <v>39507</v>
       </c>
       <c r="B93" t="n">
-        <v>3.409505687100795</v>
+        <v>3.409505541279702</v>
       </c>
       <c r="C93" t="n">
         <v>3.154947610128493</v>
       </c>
       <c r="D93" t="n">
-        <v>1.080684618705786</v>
+        <v>1.080684572615453</v>
       </c>
     </row>
     <row r="94">
@@ -1704,13 +1704,13 @@
         <v>39538</v>
       </c>
       <c r="B94" t="n">
-        <v>3.378811884185837</v>
+        <v>3.378811837312072</v>
       </c>
       <c r="C94" t="n">
         <v>3.146119038263957</v>
       </c>
       <c r="D94" t="n">
-        <v>1.073551162767841</v>
+        <v>1.073551141820803</v>
       </c>
     </row>
     <row r="95">
@@ -1718,13 +1718,13 @@
         <v>39568</v>
       </c>
       <c r="B95" t="n">
-        <v>3.368095152568174</v>
+        <v>3.368095155534408</v>
       </c>
       <c r="C95" t="n">
         <v>3.160554549910806</v>
       </c>
       <c r="D95" t="n">
-        <v>1.065682851054179</v>
+        <v>1.065682851979727</v>
       </c>
     </row>
     <row r="96">
@@ -1732,13 +1732,13 @@
         <v>39599</v>
       </c>
       <c r="B96" t="n">
-        <v>3.414093777352476</v>
+        <v>3.414093924782784</v>
       </c>
       <c r="C96" t="n">
         <v>3.148145469752225</v>
       </c>
       <c r="D96" t="n">
-        <v>1.084584758985451</v>
+        <v>1.084584805695575</v>
       </c>
     </row>
     <row r="97">
@@ -1746,13 +1746,13 @@
         <v>39629</v>
       </c>
       <c r="B97" t="n">
-        <v>3.361634806024157</v>
+        <v>3.361634833019149</v>
       </c>
       <c r="C97" t="n">
         <v>3.038966667084467</v>
       </c>
       <c r="D97" t="n">
-        <v>1.106238463613817</v>
+        <v>1.106238473053633</v>
       </c>
     </row>
     <row r="98">
@@ -1760,13 +1760,13 @@
         <v>39660</v>
       </c>
       <c r="B98" t="n">
-        <v>3.288160442741723</v>
+        <v>3.288160712565759</v>
       </c>
       <c r="C98" t="n">
         <v>3.019156507823778</v>
       </c>
       <c r="D98" t="n">
-        <v>1.089097313521713</v>
+        <v>1.089097402809474</v>
       </c>
     </row>
     <row r="99">
@@ -1774,13 +1774,13 @@
         <v>39691</v>
       </c>
       <c r="B99" t="n">
-        <v>3.323014561402723</v>
+        <v>3.323014821671469</v>
       </c>
       <c r="C99" t="n">
         <v>3.033247383017289</v>
       </c>
       <c r="D99" t="n">
-        <v>1.096584313098211</v>
+        <v>1.09658440832471</v>
       </c>
     </row>
     <row r="100">
@@ -1788,13 +1788,13 @@
         <v>39721</v>
       </c>
       <c r="B100" t="n">
-        <v>3.259950248364385</v>
+        <v>3.259950275650266</v>
       </c>
       <c r="C100" t="n">
         <v>3.07762272791429</v>
       </c>
       <c r="D100" t="n">
-        <v>1.05924567138982</v>
+        <v>1.059245680500042</v>
       </c>
     </row>
     <row r="101">
@@ -1802,13 +1802,13 @@
         <v>39752</v>
       </c>
       <c r="B101" t="n">
-        <v>3.559573518567515</v>
+        <v>3.559573515585688</v>
       </c>
       <c r="C101" t="n">
         <v>3.238386973090794</v>
       </c>
       <c r="D101" t="n">
-        <v>1.098891561549431</v>
+        <v>1.098891559827289</v>
       </c>
     </row>
     <row r="102">
@@ -1816,13 +1816,13 @@
         <v>39782</v>
       </c>
       <c r="B102" t="n">
-        <v>3.862175150653442</v>
+        <v>3.862175062057688</v>
       </c>
       <c r="C102" t="n">
         <v>3.329625010490417</v>
       </c>
       <c r="D102" t="n">
-        <v>1.160269272668475</v>
+        <v>1.160269245828125</v>
       </c>
     </row>
     <row r="103">
@@ -1830,13 +1830,13 @@
         <v>39813</v>
       </c>
       <c r="B103" t="n">
-        <v>3.648356153570253</v>
+        <v>3.648356270102353</v>
       </c>
       <c r="C103" t="n">
         <v>3.413873921269956</v>
       </c>
       <c r="D103" t="n">
-        <v>1.071520727630094</v>
+        <v>1.071520777359574</v>
       </c>
     </row>
     <row r="104">
@@ -1844,13 +1844,13 @@
         <v>39844</v>
       </c>
       <c r="B104" t="n">
-        <v>3.710487837914543</v>
+        <v>3.710487941239686</v>
       </c>
       <c r="C104" t="n">
         <v>3.453568165952509</v>
       </c>
       <c r="D104" t="n">
-        <v>1.074079316251702</v>
+        <v>1.074079348396131</v>
       </c>
     </row>
     <row r="105">
@@ -1858,13 +1858,13 @@
         <v>39872</v>
       </c>
       <c r="B105" t="n">
-        <v>3.83422891141592</v>
+        <v>3.834228979421251</v>
       </c>
       <c r="C105" t="n">
         <v>3.506929981708526</v>
       </c>
       <c r="D105" t="n">
-        <v>1.093387188251337</v>
+        <v>1.093387207747182</v>
       </c>
     </row>
     <row r="106">
@@ -1872,13 +1872,13 @@
         <v>39903</v>
       </c>
       <c r="B106" t="n">
-        <v>3.939691953423319</v>
+        <v>3.939692234857171</v>
       </c>
       <c r="C106" t="n">
         <v>3.648895447904414</v>
       </c>
       <c r="D106" t="n">
-        <v>1.079955396327815</v>
+        <v>1.079955472943769</v>
       </c>
     </row>
     <row r="107">
@@ -1886,13 +1886,13 @@
         <v>39933</v>
       </c>
       <c r="B107" t="n">
-        <v>3.884663773651044</v>
+        <v>3.884663655491382</v>
       </c>
       <c r="C107" t="n">
         <v>3.685063633051786</v>
       </c>
       <c r="D107" t="n">
-        <v>1.054132479622278</v>
+        <v>1.054132446839188</v>
       </c>
     </row>
     <row r="108">
@@ -1900,13 +1900,13 @@
         <v>39964</v>
       </c>
       <c r="B108" t="n">
-        <v>3.856334790599281</v>
+        <v>3.856334878079349</v>
       </c>
       <c r="C108" t="n">
         <v>3.71785238810948</v>
       </c>
       <c r="D108" t="n">
-        <v>1.037250795920921</v>
+        <v>1.037250819018561</v>
       </c>
     </row>
     <row r="109">
@@ -1914,13 +1914,13 @@
         <v>39994</v>
       </c>
       <c r="B109" t="n">
-        <v>3.957743716512304</v>
+        <v>3.957743900395899</v>
       </c>
       <c r="C109" t="n">
         <v>3.763850017027421</v>
       </c>
       <c r="D109" t="n">
-        <v>1.051440884333553</v>
+        <v>1.05144093273036</v>
       </c>
     </row>
     <row r="110">
@@ -1928,13 +1928,13 @@
         <v>40025</v>
       </c>
       <c r="B110" t="n">
-        <v>3.994096853259677</v>
+        <v>3.994096800801259</v>
       </c>
       <c r="C110" t="n">
         <v>3.808673931204754</v>
       </c>
       <c r="D110" t="n">
-        <v>1.048700356641092</v>
+        <v>1.048700342815196</v>
       </c>
     </row>
     <row r="111">
@@ -1942,13 +1942,13 @@
         <v>40056</v>
       </c>
       <c r="B111" t="n">
-        <v>3.923177061127452</v>
+        <v>3.923177139475425</v>
       </c>
       <c r="C111" t="n">
         <v>3.834676163537162</v>
       </c>
       <c r="D111" t="n">
-        <v>1.02308430465393</v>
+        <v>1.023084325147892</v>
       </c>
     </row>
     <row r="112">
@@ -1956,13 +1956,13 @@
         <v>40086</v>
       </c>
       <c r="B112" t="n">
-        <v>3.927660746399851</v>
+        <v>3.927660981855833</v>
       </c>
       <c r="C112" t="n">
         <v>3.826663645831021</v>
       </c>
       <c r="D112" t="n">
-        <v>1.026395037264663</v>
+        <v>1.026395098801335</v>
       </c>
     </row>
     <row r="113">
@@ -1970,13 +1970,13 @@
         <v>40117</v>
       </c>
       <c r="B113" t="n">
-        <v>3.859377825104406</v>
+        <v>3.859377852957068</v>
       </c>
       <c r="C113" t="n">
         <v>3.820095441558145</v>
       </c>
       <c r="D113" t="n">
-        <v>1.010279896799989</v>
+        <v>1.010279904050948</v>
       </c>
     </row>
     <row r="114">
@@ -1984,13 +1984,13 @@
         <v>40147</v>
       </c>
       <c r="B114" t="n">
-        <v>3.855609994222493</v>
+        <v>3.855609987340716</v>
       </c>
       <c r="C114" t="n">
         <v>3.80443811416626</v>
       </c>
       <c r="D114" t="n">
-        <v>1.013453366458127</v>
+        <v>1.013453364648973</v>
       </c>
     </row>
     <row r="115">
@@ -1998,13 +1998,13 @@
         <v>40178</v>
       </c>
       <c r="B115" t="n">
-        <v>3.842301429840346</v>
+        <v>3.842301550706127</v>
       </c>
       <c r="C115" t="n">
         <v>3.794695657232533</v>
       </c>
       <c r="D115" t="n">
-        <v>1.012415246317199</v>
+        <v>1.012415281440976</v>
       </c>
     </row>
     <row r="116">
@@ -2012,13 +2012,13 @@
         <v>40209</v>
       </c>
       <c r="B116" t="n">
-        <v>3.88332590480996</v>
+        <v>3.883325582587749</v>
       </c>
       <c r="C116" t="n">
         <v>3.793633336112613</v>
       </c>
       <c r="D116" t="n">
-        <v>1.022768036172569</v>
+        <v>1.022767954849372</v>
       </c>
     </row>
     <row r="117">
@@ -2026,13 +2026,13 @@
         <v>40237</v>
       </c>
       <c r="B117" t="n">
-        <v>3.940053252008836</v>
+        <v>3.940053430874211</v>
       </c>
       <c r="C117" t="n">
         <v>3.846555018424988</v>
       </c>
       <c r="D117" t="n">
-        <v>1.02345272900989</v>
+        <v>1.02345278021021</v>
       </c>
     </row>
     <row r="118">
@@ -2040,13 +2040,13 @@
         <v>40268</v>
       </c>
       <c r="B118" t="n">
-        <v>3.951764908843931</v>
+        <v>3.951764861341314</v>
       </c>
       <c r="C118" t="n">
         <v>3.858386951944103</v>
       </c>
       <c r="D118" t="n">
-        <v>1.024214137105286</v>
+        <v>1.024214124956319</v>
       </c>
     </row>
     <row r="119">
@@ -2054,13 +2054,13 @@
         <v>40298</v>
       </c>
       <c r="B119" t="n">
-        <v>3.950399502803701</v>
+        <v>3.950399396125756</v>
       </c>
       <c r="C119" t="n">
         <v>3.863922736861489</v>
       </c>
       <c r="D119" t="n">
-        <v>1.021786131828011</v>
+        <v>1.021786096932932</v>
       </c>
     </row>
     <row r="120">
@@ -2068,13 +2068,13 @@
         <v>40329</v>
       </c>
       <c r="B120" t="n">
-        <v>3.99703905014023</v>
+        <v>3.997038960574919</v>
       </c>
       <c r="C120" t="n">
         <v>3.889490456808181</v>
       </c>
       <c r="D120" t="n">
-        <v>1.027826240124295</v>
+        <v>1.027826217498467</v>
       </c>
     </row>
     <row r="121">
@@ -2082,13 +2082,13 @@
         <v>40359</v>
       </c>
       <c r="B121" t="n">
-        <v>4.05263396147467</v>
+        <v>4.052633786563685</v>
       </c>
       <c r="C121" t="n">
         <v>3.926413644443859</v>
       </c>
       <c r="D121" t="n">
-        <v>1.032163366033282</v>
+        <v>1.032163321465157</v>
       </c>
     </row>
     <row r="122">
@@ -2096,13 +2096,13 @@
         <v>40390</v>
       </c>
       <c r="B122" t="n">
-        <v>4.010994945963776</v>
+        <v>4.010994651269157</v>
       </c>
       <c r="C122" t="n">
         <v>3.925749984654513</v>
       </c>
       <c r="D122" t="n">
-        <v>1.021732161202176</v>
+        <v>1.021732086084554</v>
       </c>
     </row>
     <row r="123">
@@ -2110,13 +2110,13 @@
         <v>40421</v>
       </c>
       <c r="B123" t="n">
-        <v>4.004446902188397</v>
+        <v>4.004446947447265</v>
       </c>
       <c r="C123" t="n">
         <v>3.93244545026259</v>
       </c>
       <c r="D123" t="n">
-        <v>1.018328790775713</v>
+        <v>1.01832880223144</v>
       </c>
     </row>
     <row r="124">
@@ -2124,13 +2124,13 @@
         <v>40451</v>
       </c>
       <c r="B124" t="n">
-        <v>4.027703799577193</v>
+        <v>4.027703780539873</v>
       </c>
       <c r="C124" t="n">
         <v>3.945772734555331</v>
       </c>
       <c r="D124" t="n">
-        <v>1.02078936361187</v>
+        <v>1.020789358879474</v>
       </c>
     </row>
     <row r="125">
@@ -2138,13 +2138,13 @@
         <v>40482</v>
       </c>
       <c r="B125" t="n">
-        <v>3.990338133112267</v>
+        <v>3.990338211733936</v>
       </c>
       <c r="C125" t="n">
         <v>3.948080948420933</v>
       </c>
       <c r="D125" t="n">
-        <v>1.010748560165463</v>
+        <v>1.010748580232705</v>
       </c>
     </row>
     <row r="126">
@@ -2152,13 +2152,13 @@
         <v>40512</v>
       </c>
       <c r="B126" t="n">
-        <v>4.035728597942093</v>
+        <v>4.035728636368581</v>
       </c>
       <c r="C126" t="n">
         <v>3.960772763599049</v>
       </c>
       <c r="D126" t="n">
-        <v>1.018925298570821</v>
+        <v>1.018925308297399</v>
       </c>
     </row>
     <row r="127">
@@ -2166,13 +2166,13 @@
         <v>40543</v>
       </c>
       <c r="B127" t="n">
-        <v>4.096038501300568</v>
+        <v>4.096038412005114</v>
       </c>
       <c r="C127" t="n">
         <v>3.971178251764049</v>
       </c>
       <c r="D127" t="n">
-        <v>1.032054007761882</v>
+        <v>1.032053984901759</v>
       </c>
     </row>
     <row r="128">
@@ -2180,13 +2180,13 @@
         <v>40574</v>
       </c>
       <c r="B128" t="n">
-        <v>4.129950633860066</v>
+        <v>4.129950536247572</v>
       </c>
       <c r="C128" t="n">
         <v>3.96079048656282</v>
       </c>
       <c r="D128" t="n">
-        <v>1.042770711602794</v>
+        <v>1.042770687136321</v>
       </c>
     </row>
     <row r="129">
@@ -2194,13 +2194,13 @@
         <v>40602</v>
       </c>
       <c r="B129" t="n">
-        <v>4.232093743084391</v>
+        <v>4.232093743583175</v>
       </c>
       <c r="C129" t="n">
         <v>4.011280059814453</v>
       </c>
       <c r="D129" t="n">
-        <v>1.055036934743852</v>
+        <v>1.055036934875302</v>
       </c>
     </row>
     <row r="130">
@@ -2208,13 +2208,13 @@
         <v>40633</v>
       </c>
       <c r="B130" t="n">
-        <v>4.316915740296503</v>
+        <v>4.316915748121839</v>
       </c>
       <c r="C130" t="n">
         <v>4.031447845956554</v>
       </c>
       <c r="D130" t="n">
-        <v>1.070818889862594</v>
+        <v>1.070818891748776</v>
       </c>
     </row>
     <row r="131">
@@ -2222,13 +2222,13 @@
         <v>40663</v>
       </c>
       <c r="B131" t="n">
-        <v>4.346166278116031</v>
+        <v>4.346166279059834</v>
       </c>
       <c r="C131" t="n">
         <v>4.059050011634826</v>
       </c>
       <c r="D131" t="n">
-        <v>1.071047767644823</v>
+        <v>1.071047777787461</v>
       </c>
     </row>
     <row r="132">
@@ -2236,13 +2236,13 @@
         <v>40694</v>
       </c>
       <c r="B132" t="n">
-        <v>4.405055768455384</v>
+        <v>4.405055735093743</v>
       </c>
       <c r="C132" t="n">
         <v>4.080863584171642</v>
       </c>
       <c r="D132" t="n">
-        <v>1.079487100015388</v>
+        <v>1.079487091681333</v>
       </c>
     </row>
     <row r="133">
@@ -2250,13 +2250,13 @@
         <v>40724</v>
       </c>
       <c r="B133" t="n">
-        <v>4.349786260563426</v>
+        <v>4.349786147807401</v>
       </c>
       <c r="C133" t="n">
         <v>4.088731787421486</v>
       </c>
       <c r="D133" t="n">
-        <v>1.063861910293381</v>
+        <v>1.063861882678681</v>
       </c>
     </row>
     <row r="134">
@@ -2264,13 +2264,13 @@
         <v>40755</v>
       </c>
       <c r="B134" t="n">
-        <v>4.267703053609364</v>
+        <v>4.267703016514326</v>
       </c>
       <c r="C134" t="n">
         <v>4.111733300345285</v>
       </c>
       <c r="D134" t="n">
-        <v>1.037955182107491</v>
+        <v>1.037955173026987</v>
       </c>
     </row>
     <row r="135">
@@ -2278,13 +2278,13 @@
         <v>40786</v>
       </c>
       <c r="B135" t="n">
-        <v>4.399478629714706</v>
+        <v>4.399478683724763</v>
       </c>
       <c r="C135" t="n">
         <v>4.151234813358473</v>
       </c>
       <c r="D135" t="n">
-        <v>1.05985021450766</v>
+        <v>1.059850227558912</v>
       </c>
     </row>
     <row r="136">
@@ -2292,13 +2292,13 @@
         <v>40816</v>
       </c>
       <c r="B136" t="n">
-        <v>4.630045576630069</v>
+        <v>4.630045599513881</v>
       </c>
       <c r="C136" t="n">
         <v>4.205581795085561</v>
       </c>
       <c r="D136" t="n">
-        <v>1.100928749262837</v>
+        <v>1.100928754777866</v>
       </c>
     </row>
     <row r="137">
@@ -2306,13 +2306,13 @@
         <v>40847</v>
       </c>
       <c r="B137" t="n">
-        <v>4.733015418883491</v>
+        <v>4.733015468202415</v>
       </c>
       <c r="C137" t="n">
         <v>4.204066662561326</v>
       </c>
       <c r="D137" t="n">
-        <v>1.125739426288569</v>
+        <v>1.125739437868839</v>
       </c>
     </row>
     <row r="138">
@@ -2320,13 +2320,13 @@
         <v>40877</v>
       </c>
       <c r="B138" t="n">
-        <v>4.767334479937472</v>
+        <v>4.767334679208884</v>
       </c>
       <c r="C138" t="n">
         <v>4.256290912628174</v>
       </c>
       <c r="D138" t="n">
-        <v>1.120103162369871</v>
+        <v>1.120103209147806</v>
       </c>
     </row>
     <row r="139">
@@ -2334,13 +2334,13 @@
         <v>40908</v>
       </c>
       <c r="B139" t="n">
-        <v>4.746621049702426</v>
+        <v>4.746621321641181</v>
       </c>
       <c r="C139" t="n">
         <v>4.282386346296831</v>
       </c>
       <c r="D139" t="n">
-        <v>1.108719855713648</v>
+        <v>1.108719929872286</v>
       </c>
     </row>
     <row r="140">
@@ -2348,13 +2348,13 @@
         <v>40939</v>
       </c>
       <c r="B140" t="n">
-        <v>4.677996206322005</v>
+        <v>4.677996322082139</v>
       </c>
       <c r="C140" t="n">
         <v>4.313113646073774</v>
       </c>
       <c r="D140" t="n">
-        <v>1.085177823647517</v>
+        <v>1.085177847777184</v>
       </c>
     </row>
     <row r="141">
@@ -2362,13 +2362,13 @@
         <v>40968</v>
       </c>
       <c r="B141" t="n">
-        <v>4.768131425373481</v>
+        <v>4.768131394240592</v>
       </c>
       <c r="C141" t="n">
         <v>4.339452402932303</v>
       </c>
       <c r="D141" t="n">
-        <v>1.098405971420783</v>
+        <v>1.098405963473728</v>
       </c>
     </row>
     <row r="142">
@@ -2376,13 +2376,13 @@
         <v>40999</v>
       </c>
       <c r="B142" t="n">
-        <v>5.012799102523564</v>
+        <v>5.012799012962645</v>
       </c>
       <c r="C142" t="n">
         <v>4.346218195828524</v>
       </c>
       <c r="D142" t="n">
-        <v>1.153341532745297</v>
+        <v>1.153341512092351</v>
       </c>
     </row>
     <row r="143">
@@ -2390,13 +2390,13 @@
         <v>41029</v>
       </c>
       <c r="B143" t="n">
-        <v>5.471539961295215</v>
+        <v>5.471539993480173</v>
       </c>
       <c r="C143" t="n">
         <v>4.387904734838576</v>
       </c>
       <c r="D143" t="n">
-        <v>1.246216532851895</v>
+        <v>1.246216541873266</v>
       </c>
     </row>
     <row r="144">
@@ -2404,13 +2404,13 @@
         <v>41060</v>
       </c>
       <c r="B144" t="n">
-        <v>5.844391403259475</v>
+        <v>5.844391384814533</v>
       </c>
       <c r="C144" t="n">
         <v>4.43973041617352</v>
       </c>
       <c r="D144" t="n">
-        <v>1.316152936454994</v>
+        <v>1.316152932267115</v>
       </c>
     </row>
     <row r="145">
@@ -2418,13 +2418,13 @@
         <v>41090</v>
       </c>
       <c r="B145" t="n">
-        <v>6.509228954490231</v>
+        <v>6.509228810272565</v>
       </c>
       <c r="C145" t="n">
         <v>4.47493330637614</v>
       </c>
       <c r="D145" t="n">
-        <v>1.45460918887001</v>
+        <v>1.454609156902772</v>
       </c>
     </row>
     <row r="146">
@@ -2432,13 +2432,13 @@
         <v>41121</v>
       </c>
       <c r="B146" t="n">
-        <v>6.781342682424891</v>
+        <v>6.781342693075791</v>
       </c>
       <c r="C146" t="n">
         <v>4.536231864582408</v>
       </c>
       <c r="D146" t="n">
-        <v>1.494916663684819</v>
+        <v>1.494916666103725</v>
       </c>
     </row>
     <row r="147">
@@ -2446,13 +2446,13 @@
         <v>41152</v>
       </c>
       <c r="B147" t="n">
-        <v>6.557663311888696</v>
+        <v>6.557663345863065</v>
       </c>
       <c r="C147" t="n">
         <v>4.595208727795145</v>
       </c>
       <c r="D147" t="n">
-        <v>1.427120861221551</v>
+        <v>1.427120868588843</v>
       </c>
     </row>
     <row r="148">
@@ -2460,13 +2460,13 @@
         <v>41182</v>
       </c>
       <c r="B148" t="n">
-        <v>6.347426908832569</v>
+        <v>6.347427050124954</v>
       </c>
       <c r="C148" t="n">
         <v>4.66098005771637</v>
       </c>
       <c r="D148" t="n">
-        <v>1.361939348695949</v>
+        <v>1.361939379070608</v>
       </c>
     </row>
     <row r="149">
@@ -2474,13 +2474,13 @@
         <v>41213</v>
       </c>
       <c r="B149" t="n">
-        <v>6.373718642368948</v>
+        <v>6.373718548463012</v>
       </c>
       <c r="C149" t="n">
         <v>4.71827388846356</v>
       </c>
       <c r="D149" t="n">
-        <v>1.350810097136748</v>
+        <v>1.350810076984721</v>
       </c>
     </row>
     <row r="150">
@@ -2488,13 +2488,13 @@
         <v>41243</v>
       </c>
       <c r="B150" t="n">
-        <v>6.863825483917854</v>
+        <v>6.863825353160019</v>
       </c>
       <c r="C150" t="n">
         <v>4.782122785394842</v>
       </c>
       <c r="D150" t="n">
-        <v>1.435442239152058</v>
+        <v>1.435442211399528</v>
       </c>
     </row>
     <row r="151">
@@ -2502,13 +2502,13 @@
         <v>41274</v>
       </c>
       <c r="B151" t="n">
-        <v>6.652539321614126</v>
+        <v>6.652539273178705</v>
       </c>
       <c r="C151" t="n">
         <v>4.869969964027405</v>
       </c>
       <c r="D151" t="n">
-        <v>1.371101340105533</v>
+        <v>1.371101322980016</v>
       </c>
     </row>
     <row r="152">
@@ -2516,13 +2516,13 @@
         <v>41305</v>
       </c>
       <c r="B152" t="n">
-        <v>7.264060105851956</v>
+        <v>7.264060254875713</v>
       </c>
       <c r="C152" t="n">
         <v>4.940052198327106</v>
       </c>
       <c r="D152" t="n">
-        <v>1.466709585373915</v>
+        <v>1.466709614681293</v>
       </c>
     </row>
     <row r="153">
@@ -2530,13 +2530,13 @@
         <v>41333</v>
       </c>
       <c r="B153" t="n">
-        <v>7.764682554974276</v>
+        <v>7.764682864793869</v>
       </c>
       <c r="C153" t="n">
         <v>4.997624945640564</v>
       </c>
       <c r="D153" t="n">
-        <v>1.553735649625988</v>
+        <v>1.553735711521228</v>
       </c>
     </row>
     <row r="154">
@@ -2544,13 +2544,13 @@
         <v>41364</v>
       </c>
       <c r="B154" t="n">
-        <v>8.212229662131262</v>
+        <v>8.212229633247691</v>
       </c>
       <c r="C154" t="n">
         <v>5.08112857455299</v>
       </c>
       <c r="D154" t="n">
-        <v>1.617659029627384</v>
+        <v>1.617659029441735</v>
       </c>
     </row>
     <row r="155">
@@ -2558,13 +2558,13 @@
         <v>41394</v>
       </c>
       <c r="B155" t="n">
-        <v>8.712489864997117</v>
+        <v>8.712489891913169</v>
       </c>
       <c r="C155" t="n">
         <v>5.134290933609009</v>
       </c>
       <c r="D155" t="n">
-        <v>1.696742264982894</v>
+        <v>1.696742270264807</v>
       </c>
     </row>
     <row r="156">
@@ -2572,13 +2572,13 @@
         <v>41425</v>
       </c>
       <c r="B156" t="n">
-        <v>8.868435330504274</v>
+        <v>8.86843530655764</v>
       </c>
       <c r="C156" t="n">
         <v>5.219130474588145</v>
       </c>
       <c r="D156" t="n">
-        <v>1.699782417301465</v>
+        <v>1.699782412807788</v>
       </c>
     </row>
     <row r="157">
@@ -2586,13 +2586,13 @@
         <v>41455</v>
       </c>
       <c r="B157" t="n">
-        <v>8.087015307244149</v>
+        <v>8.087015216097274</v>
       </c>
       <c r="C157" t="n">
         <v>5.318244981765747</v>
       </c>
       <c r="D157" t="n">
-        <v>1.520951127565234</v>
+        <v>1.520951110247947</v>
       </c>
     </row>
     <row r="158">
@@ -2600,13 +2600,13 @@
         <v>41486</v>
       </c>
       <c r="B158" t="n">
-        <v>8.137820802159542</v>
+        <v>8.137820715340721</v>
       </c>
       <c r="C158" t="n">
         <v>5.418113045070482</v>
       </c>
       <c r="D158" t="n">
-        <v>1.501902016926496</v>
+        <v>1.501902000763162</v>
       </c>
     </row>
     <row r="159">
@@ -2614,13 +2614,13 @@
         <v>41517</v>
       </c>
       <c r="B159" t="n">
-        <v>8.524930105093334</v>
+        <v>8.524930086310578</v>
       </c>
       <c r="C159" t="n">
         <v>5.566340923309326</v>
       </c>
       <c r="D159" t="n">
-        <v>1.53146740807599</v>
+        <v>1.531467404723092</v>
       </c>
     </row>
     <row r="160">
@@ -2628,13 +2628,13 @@
         <v>41547</v>
       </c>
       <c r="B160" t="n">
-        <v>9.050599459416851</v>
+        <v>9.050599690283224</v>
       </c>
       <c r="C160" t="n">
         <v>5.723266669682094</v>
       </c>
       <c r="D160" t="n">
-        <v>1.581378243104121</v>
+        <v>1.581378283454027</v>
       </c>
     </row>
     <row r="161">
@@ -2642,13 +2642,13 @@
         <v>41578</v>
       </c>
       <c r="B161" t="n">
-        <v>9.155893355649502</v>
+        <v>9.155893287273596</v>
       </c>
       <c r="C161" t="n">
         <v>5.830922690304843</v>
       </c>
       <c r="D161" t="n">
-        <v>1.568470266946591</v>
+        <v>1.568470255823704</v>
       </c>
     </row>
     <row r="162">
@@ -2656,13 +2656,13 @@
         <v>41608</v>
       </c>
       <c r="B162" t="n">
-        <v>9.057743516145321</v>
+        <v>9.057743594591646</v>
       </c>
       <c r="C162" t="n">
         <v>6.000704765319824</v>
       </c>
       <c r="D162" t="n">
-        <v>1.510148512971468</v>
+        <v>1.510148526042613</v>
       </c>
     </row>
     <row r="163">
@@ -2670,13 +2670,13 @@
         <v>41639</v>
       </c>
       <c r="B163" t="n">
-        <v>8.487347063647896</v>
+        <v>8.487346954967588</v>
       </c>
       <c r="C163" t="n">
         <v>6.308322711424394</v>
       </c>
       <c r="D163" t="n">
-        <v>1.345348592478409</v>
+        <v>1.345348570452701</v>
       </c>
     </row>
     <row r="164">
@@ -2684,13 +2684,13 @@
         <v>41670</v>
       </c>
       <c r="B164" t="n">
-        <v>10.17063638926018</v>
+        <v>10.17063638839529</v>
       </c>
       <c r="C164" t="n">
         <v>7.00106958720995</v>
       </c>
       <c r="D164" t="n">
-        <v>1.445928594156136</v>
+        <v>1.445928594252902</v>
       </c>
     </row>
     <row r="165">
@@ -2698,13 +2698,13 @@
         <v>41698</v>
       </c>
       <c r="B165" t="n">
-        <v>10.9907347955859</v>
+        <v>10.99073497639627</v>
       </c>
       <c r="C165" t="n">
         <v>7.844880032539367</v>
       </c>
       <c r="D165" t="n">
-        <v>1.40035484581954</v>
+        <v>1.400354869020886</v>
       </c>
     </row>
     <row r="166">
@@ -2712,13 +2712,13 @@
         <v>41729</v>
       </c>
       <c r="B166" t="n">
-        <v>10.25493495036211</v>
+        <v>10.25493445001484</v>
       </c>
       <c r="C166" t="n">
         <v>7.906414259047735</v>
       </c>
       <c r="D166" t="n">
-        <v>1.297151639095191</v>
+        <v>1.29715157581799</v>
       </c>
     </row>
     <row r="167">
@@ -2726,13 +2726,13 @@
         <v>41759</v>
       </c>
       <c r="B167" t="n">
-        <v>9.795327095647703</v>
+        <v>9.795327013228231</v>
       </c>
       <c r="C167" t="n">
         <v>7.991013656963002</v>
       </c>
       <c r="D167" t="n">
-        <v>1.225791913564234</v>
+        <v>1.22579190329581</v>
       </c>
     </row>
     <row r="168">
@@ -2740,13 +2740,13 @@
         <v>41790</v>
       </c>
       <c r="B168" t="n">
-        <v>10.37110296921779</v>
+        <v>10.37110314539154</v>
       </c>
       <c r="C168" t="n">
         <v>8.026259075511586</v>
       </c>
       <c r="D168" t="n">
-        <v>1.29195088034771</v>
+        <v>1.291950902266958</v>
       </c>
     </row>
     <row r="169">
@@ -2754,13 +2754,13 @@
         <v>41820</v>
       </c>
       <c r="B169" t="n">
-        <v>10.41664814952977</v>
+        <v>10.41664807064683</v>
       </c>
       <c r="C169" t="n">
         <v>8.113961764744349</v>
       </c>
       <c r="D169" t="n">
-        <v>1.28381187740593</v>
+        <v>1.283811867702761</v>
       </c>
     </row>
     <row r="170">
@@ -2768,13 +2768,13 @@
         <v>41851</v>
       </c>
       <c r="B170" t="n">
-        <v>9.958976836267734</v>
+        <v>9.958976973898052</v>
       </c>
       <c r="C170" t="n">
         <v>8.139669542727264</v>
       </c>
       <c r="D170" t="n">
-        <v>1.223521829951733</v>
+        <v>1.223521846827947</v>
       </c>
     </row>
     <row r="171">
@@ -2782,13 +2782,13 @@
         <v>41882</v>
       </c>
       <c r="B171" t="n">
-        <v>11.47275179857278</v>
+        <v>11.47275203442213</v>
       </c>
       <c r="C171" t="n">
         <v>8.296447572253999</v>
       </c>
       <c r="D171" t="n">
-        <v>1.382146654952377</v>
+        <v>1.382146683430664</v>
       </c>
     </row>
     <row r="172">
@@ -2796,13 +2796,13 @@
         <v>41912</v>
       </c>
       <c r="B172" t="n">
-        <v>13.71488577597268</v>
+        <v>13.71488540364534</v>
       </c>
       <c r="C172" t="n">
         <v>8.398895437067205</v>
       </c>
       <c r="D172" t="n">
-        <v>1.632849597269977</v>
+        <v>1.632849553133768</v>
       </c>
     </row>
     <row r="173">
@@ -2810,13 +2810,13 @@
         <v>41943</v>
       </c>
       <c r="B173" t="n">
-        <v>13.61051234794757</v>
+        <v>13.61051255062343</v>
       </c>
       <c r="C173" t="n">
         <v>8.465247817661451</v>
       </c>
       <c r="D173" t="n">
-        <v>1.60790683614515</v>
+        <v>1.607906860072249</v>
       </c>
     </row>
     <row r="174">
@@ -2824,13 +2824,13 @@
         <v>41973</v>
       </c>
       <c r="B174" t="n">
-        <v>12.31381927370972</v>
+        <v>12.31381982182783</v>
       </c>
       <c r="C174" t="n">
         <v>8.497109985351562</v>
       </c>
       <c r="D174" t="n">
-        <v>1.449248418464737</v>
+        <v>1.449248482976622</v>
       </c>
     </row>
     <row r="175">
@@ -2838,13 +2838,13 @@
         <v>42004</v>
       </c>
       <c r="B175" t="n">
-        <v>11.49518263274697</v>
+        <v>11.49518347709918</v>
       </c>
       <c r="C175" t="n">
         <v>8.538352095562479</v>
       </c>
       <c r="D175" t="n">
-        <v>1.344211722447934</v>
+        <v>1.344211822380249</v>
       </c>
     </row>
     <row r="176">
@@ -2852,13 +2852,13 @@
         <v>42035</v>
       </c>
       <c r="B176" t="n">
-        <v>12.20971305052126</v>
+        <v>12.20971317928682</v>
       </c>
       <c r="C176" t="n">
         <v>8.586059136824174</v>
       </c>
       <c r="D176" t="n">
-        <v>1.420238819966404</v>
+        <v>1.420238841987558</v>
       </c>
     </row>
     <row r="177">
@@ -2866,13 +2866,13 @@
         <v>42063</v>
       </c>
       <c r="B177" t="n">
-        <v>12.07736481049593</v>
+        <v>12.07736452728754</v>
       </c>
       <c r="C177" t="n">
         <v>8.671775007247925</v>
       </c>
       <c r="D177" t="n">
-        <v>1.393717640926336</v>
+        <v>1.39371760548803</v>
       </c>
     </row>
     <row r="178">
@@ -2880,13 +2880,13 @@
         <v>42094</v>
       </c>
       <c r="B178" t="n">
-        <v>11.91222715450307</v>
+        <v>11.91222699857917</v>
       </c>
       <c r="C178" t="n">
         <v>8.772790908813477</v>
       </c>
       <c r="D178" t="n">
-        <v>1.357857131890408</v>
+        <v>1.357857114073041</v>
       </c>
     </row>
     <row r="179">
@@ -2894,13 +2894,13 @@
         <v>42124</v>
       </c>
       <c r="B179" t="n">
-        <v>11.91332830466785</v>
+        <v>11.91332824671242</v>
       </c>
       <c r="C179" t="n">
         <v>8.851409001783891</v>
       </c>
       <c r="D179" t="n">
-        <v>1.346757319590134</v>
+        <v>1.346757308139459</v>
       </c>
     </row>
     <row r="180">
@@ -2908,13 +2908,13 @@
         <v>42155</v>
       </c>
       <c r="B180" t="n">
-        <v>11.86908989944216</v>
+        <v>11.8690896936673</v>
       </c>
       <c r="C180" t="n">
         <v>8.949766704014369</v>
       </c>
       <c r="D180" t="n">
-        <v>1.325631562894396</v>
+        <v>1.32563153859396</v>
       </c>
     </row>
     <row r="181">
@@ -2922,13 +2922,13 @@
         <v>42185</v>
       </c>
       <c r="B181" t="n">
-        <v>12.08328720149393</v>
+        <v>12.08328690850618</v>
       </c>
       <c r="C181" t="n">
         <v>9.052922638979824</v>
       </c>
       <c r="D181" t="n">
-        <v>1.334619090691568</v>
+        <v>1.334619058353973</v>
       </c>
     </row>
     <row r="182">
@@ -2936,13 +2936,13 @@
         <v>42216</v>
       </c>
       <c r="B182" t="n">
-        <v>13.29523092851269</v>
+        <v>13.29523076672638</v>
       </c>
       <c r="C182" t="n">
         <v>9.143543450728707</v>
       </c>
       <c r="D182" t="n">
-        <v>1.454057927038541</v>
+        <v>1.454057909314188</v>
       </c>
     </row>
     <row r="183">
@@ -2950,13 +2950,13 @@
         <v>42247</v>
       </c>
       <c r="B183" t="n">
-        <v>13.50211237599214</v>
+        <v>13.5021123282343</v>
       </c>
       <c r="C183" t="n">
         <v>9.241238003685361</v>
       </c>
       <c r="D183" t="n">
-        <v>1.461033508461941</v>
+        <v>1.461033503262875</v>
       </c>
     </row>
     <row r="184">
@@ -2964,13 +2964,13 @@
         <v>42277</v>
       </c>
       <c r="B184" t="n">
-        <v>13.92871919552258</v>
+        <v>13.92871873357087</v>
       </c>
       <c r="C184" t="n">
         <v>9.358627319335938</v>
       </c>
       <c r="D184" t="n">
-        <v>1.488373154935151</v>
+        <v>1.488373105510537</v>
       </c>
     </row>
     <row r="185">
@@ -2978,13 +2978,13 @@
         <v>42308</v>
       </c>
       <c r="B185" t="n">
-        <v>13.780229828606</v>
+        <v>13.78023005110536</v>
       </c>
       <c r="C185" t="n">
         <v>9.464222821322354</v>
       </c>
       <c r="D185" t="n">
-        <v>1.456060941602176</v>
+        <v>1.456060965086661</v>
       </c>
     </row>
     <row r="186">
@@ -2992,13 +2992,13 @@
         <v>42338</v>
       </c>
       <c r="B186" t="n">
-        <v>14.32860743241238</v>
+        <v>14.32860718360764</v>
       </c>
       <c r="C186" t="n">
         <v>9.592733337765647</v>
       </c>
       <c r="D186" t="n">
-        <v>1.493575228409688</v>
+        <v>1.493575202396069</v>
       </c>
     </row>
     <row r="187">
@@ -3006,13 +3006,13 @@
         <v>42369</v>
       </c>
       <c r="B187" t="n">
-        <v>14.4102788451122</v>
+        <v>14.41027885603593</v>
       </c>
       <c r="C187" t="n">
         <v>11.13094354712445</v>
       </c>
       <c r="D187" t="n">
-        <v>1.325777148173949</v>
+        <v>1.325777150446666</v>
       </c>
     </row>
     <row r="188">
@@ -3020,13 +3020,13 @@
         <v>42400</v>
       </c>
       <c r="B188" t="n">
-        <v>13.99011918113853</v>
+        <v>13.99011975261422</v>
       </c>
       <c r="C188" t="n">
         <v>13.51314281281971</v>
       </c>
       <c r="D188" t="n">
-        <v>1.034795560338205</v>
+        <v>1.034795601486599</v>
       </c>
     </row>
     <row r="189">
@@ -3034,13 +3034,13 @@
         <v>42429</v>
       </c>
       <c r="B189" t="n">
-        <v>14.94078667228479</v>
+        <v>14.94078650578507</v>
       </c>
       <c r="C189" t="n">
         <v>14.66890471322196</v>
       </c>
       <c r="D189" t="n">
-        <v>1.018633945229564</v>
+        <v>1.018633934809205</v>
       </c>
     </row>
     <row r="190">
@@ -3048,13 +3048,13 @@
         <v>42460</v>
       </c>
       <c r="B190" t="n">
-        <v>14.90423682372445</v>
+        <v>14.90423704558791</v>
       </c>
       <c r="C190" t="n">
         <v>14.95447813946268</v>
       </c>
       <c r="D190" t="n">
-        <v>0.995719155478991</v>
+        <v>0.9957191697644642</v>
       </c>
     </row>
     <row r="191">
@@ -3062,13 +3062,13 @@
         <v>42490</v>
       </c>
       <c r="B191" t="n">
-        <v>14.37480043868547</v>
+        <v>14.37480050446298</v>
       </c>
       <c r="C191" t="n">
         <v>14.40580940246582</v>
       </c>
       <c r="D191" t="n">
-        <v>0.9979249628224599</v>
+        <v>0.9979249673837376</v>
       </c>
     </row>
     <row r="192">
@@ -3076,13 +3076,13 @@
         <v>42521</v>
       </c>
       <c r="B192" t="n">
-        <v>14.02254351995646</v>
+        <v>14.02254348702269</v>
       </c>
       <c r="C192" t="n">
         <v>14.12472724914551</v>
       </c>
       <c r="D192" t="n">
-        <v>0.9927711215854426</v>
+        <v>0.9927711192411484</v>
       </c>
     </row>
     <row r="193">
@@ -3090,13 +3090,13 @@
         <v>42551</v>
       </c>
       <c r="B193" t="n">
-        <v>14.15068875921108</v>
+        <v>14.15068853844835</v>
       </c>
       <c r="C193" t="n">
         <v>14.10331808437001</v>
       </c>
       <c r="D193" t="n">
-        <v>1.003430217755786</v>
+        <v>1.003430202704289</v>
       </c>
     </row>
     <row r="194">
@@ -3104,13 +3104,13 @@
         <v>42582</v>
       </c>
       <c r="B194" t="n">
-        <v>14.95556002956017</v>
+        <v>14.95556011141306</v>
       </c>
       <c r="C194" t="n">
         <v>14.87476189931234</v>
       </c>
       <c r="D194" t="n">
-        <v>1.005425843957403</v>
+        <v>1.005425849701856</v>
       </c>
     </row>
     <row r="195">
@@ -3118,13 +3118,13 @@
         <v>42613</v>
       </c>
       <c r="B195" t="n">
-        <v>14.86740452492335</v>
+        <v>14.86740480711666</v>
       </c>
       <c r="C195" t="n">
         <v>14.83001302636188</v>
       </c>
       <c r="D195" t="n">
-        <v>1.002527944603927</v>
+        <v>1.002527963700945</v>
       </c>
     </row>
     <row r="196">
@@ -3132,13 +3132,13 @@
         <v>42643</v>
       </c>
       <c r="B196" t="n">
-        <v>15.07940440925207</v>
+        <v>15.07940451901319</v>
       </c>
       <c r="C196" t="n">
         <v>15.08902276646007</v>
       </c>
       <c r="D196" t="n">
-        <v>0.9993728621321819</v>
+        <v>0.9993728691101288</v>
       </c>
     </row>
     <row r="197">
@@ -3146,13 +3146,13 @@
         <v>42674</v>
       </c>
       <c r="B197" t="n">
-        <v>15.13952963877526</v>
+        <v>15.13952976634623</v>
       </c>
       <c r="C197" t="n">
         <v>15.16521417526972</v>
       </c>
       <c r="D197" t="n">
-        <v>0.9983107377114238</v>
+        <v>0.998310746096858</v>
       </c>
     </row>
     <row r="198">
@@ -3160,13 +3160,13 @@
         <v>42704</v>
       </c>
       <c r="B198" t="n">
-        <v>15.35753306025145</v>
+        <v>15.35753278632115</v>
       </c>
       <c r="C198" t="n">
         <v>15.3139271736145</v>
       </c>
       <c r="D198" t="n">
-        <v>1.002838757119814</v>
+        <v>1.002838739258641</v>
       </c>
     </row>
     <row r="199">
@@ -3174,13 +3174,13 @@
         <v>42735</v>
       </c>
       <c r="B199" t="n">
-        <v>15.88631385129329</v>
+        <v>15.88631393791271</v>
       </c>
       <c r="C199" t="n">
         <v>15.84360907294533</v>
       </c>
       <c r="D199" t="n">
-        <v>1.002743468163663</v>
+        <v>1.002743473611476</v>
       </c>
     </row>
     <row r="200">
@@ -3188,13 +3188,13 @@
         <v>42766</v>
       </c>
       <c r="B200" t="n">
-        <v>15.81087538671112</v>
+        <v>15.81087492443224</v>
       </c>
       <c r="C200" t="n">
         <v>15.89813644235784</v>
       </c>
       <c r="D200" t="n">
-        <v>0.9945184574576771</v>
+        <v>0.9945184284118118</v>
       </c>
     </row>
     <row r="201">
@@ -3202,13 +3202,13 @@
         <v>42794</v>
       </c>
       <c r="B201" t="n">
-        <v>15.59071104813431</v>
+        <v>15.59071114552903</v>
       </c>
       <c r="C201" t="n">
         <v>15.58530006408691</v>
       </c>
       <c r="D201" t="n">
-        <v>1.000379009320433</v>
+        <v>1.000379015481739</v>
       </c>
     </row>
     <row r="202">
@@ -3216,13 +3216,13 @@
         <v>42825</v>
       </c>
       <c r="B202" t="n">
-        <v>15.48757508322683</v>
+        <v>15.48757547033111</v>
       </c>
       <c r="C202" t="n">
         <v>15.51747392571491</v>
       </c>
       <c r="D202" t="n">
-        <v>0.9980930781957633</v>
+        <v>0.9980931032017905</v>
       </c>
     </row>
     <row r="203">
@@ -3230,13 +3230,13 @@
         <v>42855</v>
       </c>
       <c r="B203" t="n">
-        <v>15.36806468019402</v>
+        <v>15.36806456160983</v>
       </c>
       <c r="C203" t="n">
         <v>15.31845502853394</v>
       </c>
       <c r="D203" t="n">
-        <v>1.002453222139891</v>
+        <v>1.002453216385039</v>
       </c>
     </row>
     <row r="204">
@@ -3244,13 +3244,13 @@
         <v>42886</v>
       </c>
       <c r="B204" t="n">
-        <v>15.73849327646272</v>
+        <v>15.73849365502669</v>
       </c>
       <c r="C204" t="n">
         <v>15.67249994692595</v>
       </c>
       <c r="D204" t="n">
-        <v>1.004218881794071</v>
+        <v>1.004218905792589</v>
       </c>
     </row>
     <row r="205">
@@ -3258,13 +3258,13 @@
         <v>42916</v>
       </c>
       <c r="B205" t="n">
-        <v>16.12400048377152</v>
+        <v>16.12400071998994</v>
       </c>
       <c r="C205" t="n">
         <v>16.08706816759976</v>
       </c>
       <c r="D205" t="n">
-        <v>1.002279400777786</v>
+        <v>1.002279415435515</v>
       </c>
     </row>
     <row r="206">
@@ -3272,13 +3272,13 @@
         <v>42947</v>
       </c>
       <c r="B206" t="n">
-        <v>17.13833978299802</v>
+        <v>17.13833950279847</v>
       </c>
       <c r="C206" t="n">
         <v>17.13110485076904</v>
       </c>
       <c r="D206" t="n">
-        <v>1.00066036165352</v>
+        <v>1.000660350688998</v>
       </c>
     </row>
     <row r="207">
@@ -3286,13 +3286,13 @@
         <v>42978</v>
       </c>
       <c r="B207" t="n">
-        <v>17.39901716878076</v>
+        <v>17.39901717520144</v>
       </c>
       <c r="C207" t="n">
         <v>17.40605669436247</v>
       </c>
       <c r="D207" t="n">
-        <v>0.9996385541979377</v>
+        <v>0.9996385544214136</v>
       </c>
     </row>
     <row r="208">
@@ -3300,13 +3300,13 @@
         <v>43008</v>
       </c>
       <c r="B208" t="n">
-        <v>17.20678103487555</v>
+        <v>17.20678118722969</v>
       </c>
       <c r="C208" t="n">
         <v>17.24540474301293</v>
       </c>
       <c r="D208" t="n">
-        <v>0.9977816000997043</v>
+        <v>0.9977816090637813</v>
       </c>
     </row>
     <row r="209">
@@ -3314,13 +3314,13 @@
         <v>43039</v>
       </c>
       <c r="B209" t="n">
-        <v>17.42280482345345</v>
+        <v>17.42280499242035</v>
       </c>
       <c r="C209" t="n">
         <v>17.4368182962591</v>
       </c>
       <c r="D209" t="n">
-        <v>0.9992004295683748</v>
+        <v>0.9992004392597827</v>
       </c>
     </row>
     <row r="210">
@@ -3328,13 +3328,13 @@
         <v>43069</v>
       </c>
       <c r="B210" t="n">
-        <v>17.47122403830904</v>
+        <v>17.47122382532443</v>
       </c>
       <c r="C210" t="n">
         <v>17.49374752952939</v>
       </c>
       <c r="D210" t="n">
-        <v>0.9985325809499186</v>
+        <v>0.9985325636332333</v>
       </c>
     </row>
     <row r="211">
@@ -3342,13 +3342,13 @@
         <v>43100</v>
       </c>
       <c r="B211" t="n">
-        <v>17.61602141694321</v>
+        <v>17.61602142291137</v>
       </c>
       <c r="C211" t="n">
         <v>17.62966673714774</v>
       </c>
       <c r="D211" t="n">
-        <v>1.000156771342838</v>
+        <v>1.000156768977548</v>
       </c>
     </row>
     <row r="212">
@@ -3356,13 +3356,13 @@
         <v>43131</v>
       </c>
       <c r="B212" t="n">
-        <v>19.11330135178557</v>
+        <v>19.1133017487294</v>
       </c>
       <c r="C212" t="n">
         <v>18.96871716043223</v>
       </c>
       <c r="D212" t="n">
-        <v>1.007675002244596</v>
+        <v>1.007675023505178</v>
       </c>
     </row>
     <row r="213">
@@ -3370,13 +3370,13 @@
         <v>43159</v>
       </c>
       <c r="B213" t="n">
-        <v>19.93265763312266</v>
+        <v>19.93265771976489</v>
       </c>
       <c r="C213" t="n">
         <v>19.81259984970093</v>
       </c>
       <c r="D213" t="n">
-        <v>1.00607662994354</v>
+        <v>1.006076634212223</v>
       </c>
     </row>
     <row r="214">
@@ -3384,13 +3384,13 @@
         <v>43190</v>
       </c>
       <c r="B214" t="n">
-        <v>20.23179612722696</v>
+        <v>20.23179627898277</v>
       </c>
       <c r="C214" t="n">
         <v>20.21620472994718</v>
       </c>
       <c r="D214" t="n">
-        <v>1.000544856793919</v>
+        <v>1.000544865860722</v>
       </c>
     </row>
     <row r="215">
@@ -3398,13 +3398,13 @@
         <v>43220</v>
       </c>
       <c r="B215" t="n">
-        <v>20.26869339936171</v>
+        <v>20.26869348211213</v>
       </c>
       <c r="C215" t="n">
         <v>20.2105952671596</v>
       </c>
       <c r="D215" t="n">
-        <v>1.002859335586453</v>
+        <v>1.002859339801003</v>
       </c>
     </row>
     <row r="216">
@@ -3412,13 +3412,13 @@
         <v>43251</v>
       </c>
       <c r="B216" t="n">
-        <v>23.74325826097091</v>
+        <v>23.74325923927035</v>
       </c>
       <c r="C216" t="n">
         <v>23.38458251953125</v>
       </c>
       <c r="D216" t="n">
-        <v>1.016138997459754</v>
+        <v>1.016139038530266</v>
       </c>
     </row>
     <row r="217">
@@ -3426,13 +3426,13 @@
         <v>43281</v>
       </c>
       <c r="B217" t="n">
-        <v>26.82835406059348</v>
+        <v>26.82835359859076</v>
       </c>
       <c r="C217" t="n">
         <v>26.47352354867118</v>
       </c>
       <c r="D217" t="n">
-        <v>1.013449223081685</v>
+        <v>1.01344920629864</v>
       </c>
     </row>
     <row r="218">
@@ -3440,13 +3440,13 @@
         <v>43312</v>
       </c>
       <c r="B218" t="n">
-        <v>27.60330270210775</v>
+        <v>27.6033021306378</v>
       </c>
       <c r="C218" t="n">
         <v>27.66359103809704</v>
       </c>
       <c r="D218" t="n">
-        <v>0.9978790767173188</v>
+        <v>0.997879056028092</v>
       </c>
     </row>
     <row r="219">
@@ -3454,13 +3454,13 @@
         <v>43343</v>
       </c>
       <c r="B219" t="n">
-        <v>30.30237028749455</v>
+        <v>30.30237011993787</v>
       </c>
       <c r="C219" t="n">
         <v>29.7751522893491</v>
       </c>
       <c r="D219" t="n">
-        <v>1.016975503598063</v>
+        <v>1.016975496949284</v>
       </c>
     </row>
     <row r="220">
@@ -3468,13 +3468,13 @@
         <v>43373</v>
       </c>
       <c r="B220" t="n">
-        <v>38.79124705400439</v>
+        <v>38.79124673231737</v>
       </c>
       <c r="C220" t="n">
         <v>38.40638046264648</v>
       </c>
       <c r="D220" t="n">
-        <v>1.010134010801955</v>
+        <v>1.010134002453815</v>
       </c>
     </row>
     <row r="221">
@@ -3482,13 +3482,13 @@
         <v>43404</v>
       </c>
       <c r="B221" t="n">
-        <v>37.1586388761343</v>
+        <v>37.15863862205258</v>
       </c>
       <c r="C221" t="n">
         <v>37.27614361306895</v>
       </c>
       <c r="D221" t="n">
-        <v>0.9972617526348376</v>
+        <v>0.9972617457595879</v>
       </c>
     </row>
     <row r="222">
@@ -3496,13 +3496,13 @@
         <v>43434</v>
       </c>
       <c r="B222" t="n">
-        <v>36.4541305355205</v>
+        <v>36.45413036092163</v>
       </c>
       <c r="C222" t="n">
         <v>36.36993650956587</v>
       </c>
       <c r="D222" t="n">
-        <v>1.002426862324923</v>
+        <v>1.002426857456184</v>
       </c>
     </row>
     <row r="223">
@@ -3510,13 +3510,13 @@
         <v>43465</v>
       </c>
       <c r="B223" t="n">
-        <v>37.78105089761612</v>
+        <v>37.78104964670802</v>
       </c>
       <c r="C223" t="n">
         <v>37.80243810017904</v>
       </c>
       <c r="D223" t="n">
-        <v>0.99961739500598</v>
+        <v>0.9996173616115356</v>
       </c>
     </row>
     <row r="224">
@@ -3524,13 +3524,13 @@
         <v>43496</v>
       </c>
       <c r="B224" t="n">
-        <v>37.29975087198193</v>
+        <v>37.29975108543362</v>
       </c>
       <c r="C224" t="n">
         <v>37.41604332301927</v>
       </c>
       <c r="D224" t="n">
-        <v>0.9966633881506149</v>
+        <v>0.9966633923630732</v>
       </c>
     </row>
     <row r="225">
@@ -3538,13 +3538,13 @@
         <v>43524</v>
       </c>
       <c r="B225" t="n">
-        <v>38.48015866444076</v>
+        <v>38.48015819851133</v>
       </c>
       <c r="C225" t="n">
         <v>38.3035099029541</v>
       </c>
       <c r="D225" t="n">
-        <v>1.004607299694222</v>
+        <v>1.004607287144032</v>
       </c>
     </row>
     <row r="226">
@@ -3552,13 +3552,13 @@
         <v>43555</v>
       </c>
       <c r="B226" t="n">
-        <v>41.40320178038997</v>
+        <v>41.40320224056966</v>
       </c>
       <c r="C226" t="n">
         <v>41.10428074428013</v>
       </c>
       <c r="D226" t="n">
-        <v>1.007429691528866</v>
+        <v>1.007429702476905</v>
       </c>
     </row>
     <row r="227">
@@ -3566,13 +3566,13 @@
         <v>43585</v>
       </c>
       <c r="B227" t="n">
-        <v>43.30558450954663</v>
+        <v>43.30558460930016</v>
       </c>
       <c r="C227" t="n">
         <v>42.96184123646129</v>
       </c>
       <c r="D227" t="n">
-        <v>1.007527446243888</v>
+        <v>1.007527446668222</v>
       </c>
     </row>
     <row r="228">
@@ -3580,13 +3580,13 @@
         <v>43616</v>
       </c>
       <c r="B228" t="n">
-        <v>45.06184656262101</v>
+        <v>45.06184694074959</v>
       </c>
       <c r="C228" t="n">
         <v>44.83897313204679</v>
       </c>
       <c r="D228" t="n">
-        <v>1.004766168817047</v>
+        <v>1.00476617599045</v>
       </c>
     </row>
     <row r="229">
@@ -3594,13 +3594,13 @@
         <v>43646</v>
       </c>
       <c r="B229" t="n">
-        <v>43.66226452835512</v>
+        <v>43.66226425886816</v>
       </c>
       <c r="C229" t="n">
         <v>43.79814453125</v>
       </c>
       <c r="D229" t="n">
-        <v>0.9969879867089685</v>
+        <v>0.9969879801503341</v>
       </c>
     </row>
     <row r="230">
@@ -3608,13 +3608,13 @@
         <v>43677</v>
       </c>
       <c r="B230" t="n">
-        <v>42.53469044574879</v>
+        <v>42.53469070303301</v>
       </c>
       <c r="C230" t="n">
         <v>42.42439070991848</v>
       </c>
       <c r="D230" t="n">
-        <v>1.002584039158853</v>
+        <v>1.002584045502486</v>
       </c>
     </row>
     <row r="231">
@@ -3622,13 +3622,13 @@
         <v>43708</v>
       </c>
       <c r="B231" t="n">
-        <v>53.66443507906213</v>
+        <v>53.66443554082574</v>
       </c>
       <c r="C231" t="n">
         <v>51.97312251004305</v>
       </c>
       <c r="D231" t="n">
-        <v>1.032925777956627</v>
+        <v>1.03292578504633</v>
       </c>
     </row>
     <row r="232">
@@ -3636,13 +3636,13 @@
         <v>43738</v>
       </c>
       <c r="B232" t="n">
-        <v>66.08104015466668</v>
+        <v>66.08104056882289</v>
       </c>
       <c r="C232" t="n">
         <v>56.62937127976191</v>
       </c>
       <c r="D232" t="n">
-        <v>1.16749682181014</v>
+        <v>1.167496828927221</v>
       </c>
     </row>
     <row r="233">
@@ -3650,13 +3650,13 @@
         <v>43769</v>
       </c>
       <c r="B233" t="n">
-        <v>72.2336158511835</v>
+        <v>72.23361499798402</v>
       </c>
       <c r="C233" t="n">
         <v>58.34081517095151</v>
       </c>
       <c r="D233" t="n">
-        <v>1.237304995192239</v>
+        <v>1.237304980559165</v>
       </c>
     </row>
     <row r="234">
@@ -3664,13 +3664,13 @@
         <v>43799</v>
       </c>
       <c r="B234" t="n">
-        <v>76.50613224038939</v>
+        <v>76.50613168954436</v>
       </c>
       <c r="C234" t="n">
         <v>59.64329238164993</v>
       </c>
       <c r="D234" t="n">
-        <v>1.282764986644545</v>
+        <v>1.282764977413478</v>
       </c>
     </row>
     <row r="235">
@@ -3678,13 +3678,13 @@
         <v>43830</v>
       </c>
       <c r="B235" t="n">
-        <v>74.85964203884119</v>
+        <v>74.85964281306818</v>
       </c>
       <c r="C235" t="n">
         <v>59.78457919034091</v>
       </c>
       <c r="D235" t="n">
-        <v>1.250252550720409</v>
+        <v>1.25025256262455</v>
       </c>
     </row>
     <row r="236">
@@ -3692,13 +3692,13 @@
         <v>43861</v>
       </c>
       <c r="B236" t="n">
-        <v>81.19636400426317</v>
+        <v>81.19636320605015</v>
       </c>
       <c r="C236" t="n">
         <v>59.91140431943147</v>
       </c>
       <c r="D236" t="n">
-        <v>1.350418586207221</v>
+        <v>1.350418574664294</v>
       </c>
     </row>
     <row r="237">
@@ -3706,13 +3706,13 @@
         <v>43890</v>
       </c>
       <c r="B237" t="n">
-        <v>82.70814040494122</v>
+        <v>82.70813972432605</v>
       </c>
       <c r="C237" t="n">
         <v>61.23162403106689</v>
       </c>
       <c r="D237" t="n">
-        <v>1.35105023522872</v>
+        <v>1.35105022396808</v>
       </c>
     </row>
     <row r="238">
@@ -3720,13 +3720,13 @@
         <v>43921</v>
       </c>
       <c r="B238" t="n">
-        <v>87.00059676748371</v>
+        <v>87.00059803111886</v>
       </c>
       <c r="C238" t="n">
         <v>63.02305863120339</v>
       </c>
       <c r="D238" t="n">
-        <v>1.380389002440955</v>
+        <v>1.380389022268619</v>
       </c>
     </row>
     <row r="239">
@@ -3734,13 +3734,13 @@
         <v>43951</v>
       </c>
       <c r="B239" t="n">
-        <v>103.5994455232007</v>
+        <v>103.5994445103335</v>
       </c>
       <c r="C239" t="n">
         <v>65.46648649735884</v>
       </c>
       <c r="D239" t="n">
-        <v>1.577503125983616</v>
+        <v>1.57750310924839</v>
       </c>
     </row>
     <row r="240">
@@ -3748,13 +3748,13 @@
         <v>43982</v>
       </c>
       <c r="B240" t="n">
-        <v>118.3120776951105</v>
+        <v>118.3120786195001</v>
       </c>
       <c r="C240" t="n">
         <v>67.55839938209171</v>
       </c>
       <c r="D240" t="n">
-        <v>1.749446720209706</v>
+        <v>1.749446734669415</v>
       </c>
     </row>
     <row r="241">
@@ -3762,13 +3762,13 @@
         <v>44012</v>
       </c>
       <c r="B241" t="n">
-        <v>112.3771631726029</v>
+        <v>112.3771648674066</v>
       </c>
       <c r="C241" t="n">
         <v>69.39054558493875</v>
       </c>
       <c r="D241" t="n">
-        <v>1.619996882119591</v>
+        <v>1.619996906972077</v>
       </c>
     </row>
     <row r="242">
@@ -3776,13 +3776,13 @@
         <v>44043</v>
       </c>
       <c r="B242" t="n">
-        <v>114.0242210242607</v>
+        <v>114.0242238038187</v>
       </c>
       <c r="C242" t="n">
         <v>71.29541911249575</v>
       </c>
       <c r="D242" t="n">
-        <v>1.598982806728749</v>
+        <v>1.598982845560609</v>
       </c>
     </row>
     <row r="243">
@@ -3790,13 +3790,13 @@
         <v>44074</v>
       </c>
       <c r="B243" t="n">
-        <v>127.993857418323</v>
+        <v>127.9938567793605</v>
       </c>
       <c r="C243" t="n">
         <v>73.16012609572638</v>
       </c>
       <c r="D243" t="n">
-        <v>1.74941064888037</v>
+        <v>1.749410639978529</v>
       </c>
     </row>
     <row r="244">
@@ -3804,13 +3804,13 @@
         <v>44104</v>
       </c>
       <c r="B244" t="n">
-        <v>133.9211395759625</v>
+        <v>133.9211404452815</v>
       </c>
       <c r="C244" t="n">
         <v>75.06492718783292</v>
       </c>
       <c r="D244" t="n">
-        <v>1.783289932304092</v>
+        <v>1.783289944010667</v>
       </c>
     </row>
     <row r="245">
@@ -3818,13 +3818,13 @@
         <v>44135</v>
       </c>
       <c r="B245" t="n">
-        <v>161.308707510401</v>
+        <v>161.3087080601273</v>
       </c>
       <c r="C245" t="n">
         <v>77.43708523837003</v>
       </c>
       <c r="D245" t="n">
-        <v>2.082731826370667</v>
+        <v>2.082731833588565</v>
       </c>
     </row>
     <row r="246">
@@ -3832,13 +3832,13 @@
         <v>44165</v>
       </c>
       <c r="B246" t="n">
-        <v>149.5040046165172</v>
+        <v>149.5040054144293</v>
       </c>
       <c r="C246" t="n">
         <v>79.73074195498512</v>
       </c>
       <c r="D246" t="n">
-        <v>1.875373785831776</v>
+        <v>1.8753737957957</v>
       </c>
     </row>
     <row r="247">
@@ -3846,13 +3846,13 @@
         <v>44196</v>
       </c>
       <c r="B247" t="n">
-        <v>142.4779037038132</v>
+        <v>142.4779012921033</v>
       </c>
       <c r="C247" t="n">
         <v>82.51180333676545</v>
       </c>
       <c r="D247" t="n">
-        <v>1.72736916509811</v>
+        <v>1.727369134581208</v>
       </c>
     </row>
     <row r="248">
@@ -3860,13 +3860,13 @@
         <v>44227</v>
       </c>
       <c r="B248" t="n">
-        <v>151.1281035028433</v>
+        <v>151.1281040587026</v>
       </c>
       <c r="C248" t="n">
         <v>85.73309108189174</v>
       </c>
       <c r="D248" t="n">
-        <v>1.758838306423065</v>
+        <v>1.758838309980872</v>
       </c>
     </row>
     <row r="249">
@@ -3874,13 +3874,13 @@
         <v>44255</v>
       </c>
       <c r="B249" t="n">
-        <v>149.0032724728347</v>
+        <v>149.0032744229899</v>
       </c>
       <c r="C249" t="n">
         <v>88.49104499816895</v>
       </c>
       <c r="D249" t="n">
-        <v>1.68317518032621</v>
+        <v>1.683175197734611</v>
       </c>
     </row>
     <row r="250">
@@ -3888,13 +3888,13 @@
         <v>44286</v>
       </c>
       <c r="B250" t="n">
-        <v>148.6894636540233</v>
+        <v>148.6894661058273</v>
       </c>
       <c r="C250" t="n">
         <v>90.94231746507728</v>
       </c>
       <c r="D250" t="n">
-        <v>1.635245316781133</v>
+        <v>1.635245343770042</v>
       </c>
     </row>
     <row r="251">
@@ -3902,13 +3902,13 @@
         <v>44316</v>
       </c>
       <c r="B251" t="n">
-        <v>150.9099408219996</v>
+        <v>150.9099422122398</v>
       </c>
       <c r="C251" t="n">
         <v>92.62295497547497</v>
       </c>
       <c r="D251" t="n">
-        <v>1.626348424553727</v>
+        <v>1.626348438838735</v>
       </c>
     </row>
     <row r="252">
@@ -3916,13 +3916,13 @@
         <v>44347</v>
       </c>
       <c r="B252" t="n">
-        <v>159.9039792141625</v>
+        <v>159.9039811563212</v>
       </c>
       <c r="C252" t="n">
         <v>93.99819365001861</v>
       </c>
       <c r="D252" t="n">
-        <v>1.701072928642598</v>
+        <v>1.701072949138589</v>
       </c>
     </row>
     <row r="253">
@@ -3930,13 +3930,13 @@
         <v>44377</v>
       </c>
       <c r="B253" t="n">
-        <v>166.1072379991798</v>
+        <v>166.1072385840761</v>
       </c>
       <c r="C253" t="n">
         <v>95.15197545831853</v>
       </c>
       <c r="D253" t="n">
-        <v>1.745681907258749</v>
+        <v>1.745681913385203</v>
       </c>
     </row>
     <row r="254">
@@ -3944,13 +3944,13 @@
         <v>44408</v>
       </c>
       <c r="B254" t="n">
-        <v>176.0963296755454</v>
+        <v>176.0963335073425</v>
       </c>
       <c r="C254" t="n">
         <v>96.13683977994052</v>
       </c>
       <c r="D254" t="n">
-        <v>1.831654548312204</v>
+        <v>1.831654588202055</v>
       </c>
     </row>
     <row r="255">
@@ -3958,13 +3958,13 @@
         <v>44439</v>
       </c>
       <c r="B255" t="n">
-        <v>177.026095561874</v>
+        <v>177.0260981581341</v>
       </c>
       <c r="C255" t="n">
         <v>97.12412782148881</v>
       </c>
       <c r="D255" t="n">
-        <v>1.822719114719638</v>
+        <v>1.822719141522338</v>
       </c>
     </row>
     <row r="256">
@@ -3972,13 +3972,13 @@
         <v>44469</v>
       </c>
       <c r="B256" t="n">
-        <v>183.0234430113694</v>
+        <v>183.0234405242972</v>
       </c>
       <c r="C256" t="n">
         <v>98.17553572221236</v>
       </c>
       <c r="D256" t="n">
-        <v>1.864076982372585</v>
+        <v>1.864076956994059</v>
       </c>
     </row>
     <row r="257">
@@ -3986,13 +3986,13 @@
         <v>44500</v>
       </c>
       <c r="B257" t="n">
-        <v>196.1048399286126</v>
+        <v>196.1048385968756</v>
       </c>
       <c r="C257" t="n">
         <v>99.11867959158761</v>
       </c>
       <c r="D257" t="n">
-        <v>1.978365908927807</v>
+        <v>1.978365895389524</v>
       </c>
     </row>
     <row r="258">
@@ -4000,13 +4000,13 @@
         <v>44530</v>
       </c>
       <c r="B258" t="n">
-        <v>215.3317179810594</v>
+        <v>215.331719631966</v>
       </c>
       <c r="C258" t="n">
         <v>100.2537533153187</v>
       </c>
       <c r="D258" t="n">
-        <v>2.147896023391025</v>
+        <v>2.147896039866444</v>
       </c>
     </row>
     <row r="259">
@@ -4014,13 +4014,13 @@
         <v>44561</v>
       </c>
       <c r="B259" t="n">
-        <v>208.6513921793342</v>
+        <v>208.6513905657116</v>
       </c>
       <c r="C259" t="n">
         <v>101.808979531993</v>
       </c>
       <c r="D259" t="n">
-        <v>2.048525188440228</v>
+        <v>2.048525168187432</v>
       </c>
     </row>
     <row r="260">
@@ -4028,13 +4028,13 @@
         <v>44592</v>
       </c>
       <c r="B260" t="n">
-        <v>214.2938662469903</v>
+        <v>214.2938647923698</v>
       </c>
       <c r="C260" t="n">
         <v>103.8145922706241</v>
       </c>
       <c r="D260" t="n">
-        <v>2.063874788934404</v>
+        <v>2.063874774871464</v>
       </c>
     </row>
     <row r="261">
@@ -4042,13 +4042,13 @@
         <v>44620</v>
       </c>
       <c r="B261" t="n">
-        <v>211.8485212240872</v>
+        <v>211.848514775299</v>
       </c>
       <c r="C261" t="n">
         <v>106.2315074920654</v>
       </c>
       <c r="D261" t="n">
-        <v>1.994770765117843</v>
+        <v>1.99477070434251</v>
       </c>
     </row>
     <row r="262">
@@ -4056,13 +4056,13 @@
         <v>44651</v>
       </c>
       <c r="B262" t="n">
-        <v>196.0579637882898</v>
+        <v>196.0579629249494</v>
       </c>
       <c r="C262" t="n">
         <v>109.3085002069888</v>
       </c>
       <c r="D262" t="n">
-        <v>1.793990140378492</v>
+        <v>1.793990132293693</v>
       </c>
     </row>
     <row r="263">
@@ -4070,13 +4070,13 @@
         <v>44681</v>
       </c>
       <c r="B263" t="n">
-        <v>195.8417820772931</v>
+        <v>195.8417803557059</v>
       </c>
       <c r="C263" t="n">
         <v>113.1504527500698</v>
       </c>
       <c r="D263" t="n">
-        <v>1.727361302220139</v>
+        <v>1.727361288075139</v>
       </c>
     </row>
     <row r="264">
@@ -4084,13 +4084,13 @@
         <v>44712</v>
       </c>
       <c r="B264" t="n">
-        <v>209.2567477954082</v>
+        <v>209.2567446829129</v>
       </c>
       <c r="C264" t="n">
         <v>117.6256297718395</v>
       </c>
       <c r="D264" t="n">
-        <v>1.779156429225645</v>
+        <v>1.779156402481896</v>
       </c>
     </row>
     <row r="265">
@@ -4098,13 +4098,13 @@
         <v>44742</v>
       </c>
       <c r="B265" t="n">
-        <v>230.7845953919849</v>
+        <v>230.7845934613528</v>
       </c>
       <c r="C265" t="n">
         <v>122.5586700439453</v>
       </c>
       <c r="D265" t="n">
-        <v>1.885824360933724</v>
+        <v>1.885824349074571</v>
       </c>
     </row>
     <row r="266">
@@ -4112,13 +4112,13 @@
         <v>44773</v>
       </c>
       <c r="B266" t="n">
-        <v>301.7860666705764</v>
+        <v>301.786066863312</v>
       </c>
       <c r="C266" t="n">
         <v>128.0542384556362</v>
       </c>
       <c r="D266" t="n">
-        <v>2.355275952498482</v>
+        <v>2.35527595403258</v>
       </c>
     </row>
     <row r="267">
@@ -4126,13 +4126,13 @@
         <v>44804</v>
       </c>
       <c r="B267" t="n">
-        <v>290.0410926126834</v>
+        <v>290.0410997408794</v>
       </c>
       <c r="C267" t="n">
         <v>134.974385800569</v>
       </c>
       <c r="D267" t="n">
-        <v>2.149003355784924</v>
+        <v>2.149003408512654</v>
       </c>
     </row>
     <row r="268">
@@ -4140,13 +4140,13 @@
         <v>44834</v>
       </c>
       <c r="B268" t="n">
-        <v>296.0114505902052</v>
+        <v>296.0114471335183</v>
       </c>
       <c r="C268" t="n">
         <v>142.8913303722035</v>
       </c>
       <c r="D268" t="n">
-        <v>2.071032554687605</v>
+        <v>2.071032530855329</v>
       </c>
     </row>
     <row r="269">
@@ -4154,13 +4154,13 @@
         <v>44865</v>
       </c>
       <c r="B269" t="n">
-        <v>306.9971951935332</v>
+        <v>306.997197831917</v>
       </c>
       <c r="C269" t="n">
         <v>151.8414757138207</v>
       </c>
       <c r="D269" t="n">
-        <v>2.022583746985898</v>
+        <v>2.022583764637755</v>
       </c>
     </row>
     <row r="270">
@@ -4168,13 +4168,13 @@
         <v>44895</v>
       </c>
       <c r="B270" t="n">
-        <v>316.6456813368102</v>
+        <v>316.6456796474343</v>
       </c>
       <c r="C270" t="n">
         <v>161.6809727061878</v>
       </c>
       <c r="D270" t="n">
-        <v>1.958167556829184</v>
+        <v>1.958167546259888</v>
       </c>
     </row>
     <row r="271">
@@ -4182,13 +4182,13 @@
         <v>44926</v>
       </c>
       <c r="B271" t="n">
-        <v>333.4200449039475</v>
+        <v>333.4200462732069</v>
       </c>
       <c r="C271" t="n">
         <v>172.0755927345969</v>
       </c>
       <c r="D271" t="n">
-        <v>1.937934760095841</v>
+        <v>1.937934768746543</v>
       </c>
     </row>
     <row r="272">
@@ -4196,13 +4196,13 @@
         <v>44957</v>
       </c>
       <c r="B272" t="n">
-        <v>352.0839313038973</v>
+        <v>352.0839308379246</v>
       </c>
       <c r="C272" t="n">
         <v>181.7483416470614</v>
       </c>
       <c r="D272" t="n">
-        <v>1.936749458155872</v>
+        <v>1.93674945549998</v>
       </c>
     </row>
     <row r="273">
@@ -4210,13 +4210,13 @@
         <v>44985</v>
       </c>
       <c r="B273" t="n">
-        <v>366.8514684957915</v>
+        <v>366.8514706037427</v>
       </c>
       <c r="C273" t="n">
         <v>191.4259643554688</v>
       </c>
       <c r="D273" t="n">
-        <v>1.916996642715633</v>
+        <v>1.91699665118493</v>
       </c>
     </row>
     <row r="274">
@@ -4224,13 +4224,13 @@
         <v>45016</v>
       </c>
       <c r="B274" t="n">
-        <v>389.3762539705795</v>
+        <v>389.3762566260199</v>
       </c>
       <c r="C274" t="n">
         <v>202.4838794210683</v>
       </c>
       <c r="D274" t="n">
-        <v>1.922943216305357</v>
+        <v>1.922943229978501</v>
       </c>
     </row>
     <row r="275">
@@ -4238,13 +4238,13 @@
         <v>45046</v>
       </c>
       <c r="B275" t="n">
-        <v>425.9470517658431</v>
+        <v>425.9470585579011</v>
       </c>
       <c r="C275" t="n">
         <v>215.3233131408691</v>
       </c>
       <c r="D275" t="n">
-        <v>1.971763896762767</v>
+        <v>1.971763931461526</v>
       </c>
     </row>
     <row r="276">
@@ -4252,13 +4252,13 @@
         <v>45077</v>
       </c>
       <c r="B276" t="n">
-        <v>474.0035706032207</v>
+        <v>474.0035745764326</v>
       </c>
       <c r="C276" t="n">
         <v>230.4160594110903</v>
       </c>
       <c r="D276" t="n">
-        <v>2.056723855421994</v>
+        <v>2.056723873249228</v>
       </c>
     </row>
     <row r="277">
@@ -4266,13 +4266,13 @@
         <v>45107</v>
       </c>
       <c r="B277" t="n">
-        <v>504.2066256739125</v>
+        <v>504.2066289026329</v>
       </c>
       <c r="C277" t="n">
         <v>247.984055259011</v>
       </c>
       <c r="D277" t="n">
-        <v>2.034506144145559</v>
+        <v>2.0345061588441</v>
       </c>
     </row>
     <row r="278">
@@ -4280,13 +4280,13 @@
         <v>45138</v>
       </c>
       <c r="B278" t="n">
-        <v>532.6039811126104</v>
+        <v>532.6039788784577</v>
       </c>
       <c r="C278" t="n">
         <v>265.2162017822266</v>
       </c>
       <c r="D278" t="n">
-        <v>2.008256720864314</v>
+        <v>2.008256712408074</v>
       </c>
     </row>
     <row r="279">
@@ -4294,13 +4294,13 @@
         <v>45169</v>
       </c>
       <c r="B279" t="n">
-        <v>684.7375916202748</v>
+        <v>684.7375910468031</v>
       </c>
       <c r="C279" t="n">
         <v>319.9336667268173</v>
       </c>
       <c r="D279" t="n">
-        <v>2.136984883803299</v>
+        <v>2.136984881735879</v>
       </c>
     </row>
     <row r="280">
@@ -4322,13 +4322,27 @@
         <v>45230</v>
       </c>
       <c r="B281" t="n">
-        <v>933.1984993737648</v>
+        <v>922.0218874038626</v>
       </c>
       <c r="C281" t="n">
-        <v>350.0665492007607</v>
+        <v>350.0307436856356</v>
       </c>
       <c r="D281" t="n">
-        <v>2.66352271884188</v>
+        <v>2.634150865004143</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B282" t="n">
+        <v>883.0290581732406</v>
+      </c>
+      <c r="C282" t="n">
+        <v>350.9291305541992</v>
+      </c>
+      <c r="D282" t="n">
+        <v>2.523513390179599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>